<commit_message>
Add Alpine launch time
</commit_message>
<xml_diff>
--- a/f1/F1.xlsx
+++ b/f1/F1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin/projects/calendars/f1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0E0B2B9-788C-1F43-8E07-111D1FC06928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E216C6B5-B73E-5B46-AE88-79676EE3010C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3440" yWindow="780" windowWidth="28040" windowHeight="17440" xr2:uid="{65D0735D-D923-6F47-A559-767DB601EBAB}"/>
   </bookViews>
@@ -1205,11 +1205,15 @@
       <c r="D11" s="4">
         <v>44973</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="5">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="F11" s="4">
         <v>44973</v>
       </c>
-      <c r="G11" s="3"/>
+      <c r="G11" s="5">
+        <v>0.8125</v>
+      </c>
       <c r="H11"/>
       <c r="I11" t="str">
         <f>VLOOKUP(A11,Table1[],2)</f>

</xml_diff>

<commit_message>
Update Sprint race-related details
</commit_message>
<xml_diff>
--- a/f1/F1.xlsx
+++ b/f1/F1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin/projects/calendars/f1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{11D47BF8-2CD9-1D41-B86D-3CEE76C8CDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B6932B8-A661-7443-9DF9-F8535BAE0728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3440" yWindow="780" windowWidth="28040" windowHeight="17440" xr2:uid="{65D0735D-D923-6F47-A559-767DB601EBAB}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <definedName name="circuits">Data!$B$2:$B$26</definedName>
     <definedName name="countries">Data!$A$2:$A$26</definedName>
     <definedName name="locations">Data!$A$2:$D$26</definedName>
-    <definedName name="sessions">Data!$F$2:$F$9</definedName>
+    <definedName name="sessions">Data!$F$2:$F$10</definedName>
     <definedName name="teams">Data!$H$1:$H$11</definedName>
     <definedName name="timezones">Data!$D$2:$D$26</definedName>
     <definedName name="titles">Data!$C$2:$C$26</definedName>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="142">
   <si>
     <t>Country</t>
   </si>
@@ -467,6 +467,9 @@
   </si>
   <si>
     <t>11;55</t>
+  </si>
+  <si>
+    <t>Sprint Shootout</t>
   </si>
 </sst>
 </file>
@@ -625,8 +628,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A43779E-EF45-6F4C-AA64-6ABE459227DF}" name="Table2" displayName="Table2" ref="F1:F9" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="F1:F9" xr:uid="{6A43779E-EF45-6F4C-AA64-6ABE459227DF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A43779E-EF45-6F4C-AA64-6ABE459227DF}" name="Table2" displayName="Table2" ref="F1:F10" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="F1:F10" xr:uid="{6A43779E-EF45-6F4C-AA64-6ABE459227DF}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{6838BDA8-0FE3-1349-B73D-51B1D44575E4}" name="Sessions"/>
   </tableColumns>
@@ -946,12 +949,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A264AA3C-A8BA-6F48-8FC0-C3E78D3BD742}">
   <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="4"/>
     <col min="5" max="7" width="10.83203125" style="3"/>
@@ -1831,7 +1836,7 @@
         <v>96</v>
       </c>
       <c r="C30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="C30" si="24">VLOOKUP(A30,locations,4)</f>
         <v>Asia/Baku</v>
       </c>
       <c r="D30" s="4">
@@ -1841,7 +1846,7 @@
         <v>0.5625</v>
       </c>
       <c r="F30" s="4">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="F30" si="25">D30</f>
         <v>45044</v>
       </c>
       <c r="G30" s="5">
@@ -1849,11 +1854,11 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="H30" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="H30" si="26">VLOOKUP(A30,locations,2)</f>
         <v>Baku City Circuit</v>
       </c>
       <c r="I30" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" ref="I30" si="27">VLOOKUP(A30,locations,3)</f>
         <v>Azerbaijan Grand Prix</v>
       </c>
     </row>
@@ -1879,7 +1884,7 @@
         <v>45044</v>
       </c>
       <c r="G31" s="5">
-        <f t="shared" ref="G31:G33" si="24">E31+(1/24)</f>
+        <f>E31+(1/24)</f>
         <v>0.75</v>
       </c>
       <c r="H31" t="str">
@@ -1896,7 +1901,7 @@
         <v>42</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>97</v>
+        <v>141</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="1"/>
@@ -1906,15 +1911,15 @@
         <v>45045</v>
       </c>
       <c r="E32" s="5">
-        <v>0.5625</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="F32" s="4">
         <f t="shared" si="15"/>
         <v>45045</v>
       </c>
       <c r="G32" s="5">
-        <f t="shared" si="24"/>
-        <v>0.60416666666666663</v>
+        <f>E32+(3*(1/96))</f>
+        <v>0.55208333333333337</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="22"/>
@@ -1933,7 +1938,7 @@
         <v>88</v>
       </c>
       <c r="C33" t="str">
-        <f t="shared" ref="C33:C39" si="25">VLOOKUP(A33,locations,4)</f>
+        <f t="shared" si="1"/>
         <v>Asia/Baku</v>
       </c>
       <c r="D33" s="4">
@@ -1943,19 +1948,19 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="F33" s="4">
-        <f t="shared" ref="F33:F41" si="26">D33</f>
+        <f t="shared" si="15"/>
         <v>45045</v>
       </c>
       <c r="G33" s="5">
-        <f t="shared" si="24"/>
-        <v>0.77083333333333326</v>
+        <f>E33+(1/48)</f>
+        <v>0.75</v>
       </c>
       <c r="H33" t="str">
-        <f t="shared" ref="H33:H38" si="27">VLOOKUP(A33,locations,2)</f>
+        <f t="shared" si="22"/>
         <v>Baku City Circuit</v>
       </c>
       <c r="I33" t="str">
-        <f t="shared" ref="I33:I38" si="28">VLOOKUP(A33,locations,3)</f>
+        <f t="shared" si="23"/>
         <v>Azerbaijan Grand Prix</v>
       </c>
     </row>
@@ -1967,7 +1972,7 @@
         <v>10</v>
       </c>
       <c r="C34" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" ref="C34:C39" si="28">VLOOKUP(A34,locations,4)</f>
         <v>Asia/Baku</v>
       </c>
       <c r="D34" s="4">
@@ -1977,19 +1982,19 @@
         <v>0.625</v>
       </c>
       <c r="F34" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" ref="F34:F41" si="29">D34</f>
         <v>45046</v>
       </c>
       <c r="G34" s="5">
-        <f t="shared" ref="G34" si="29">E34+(2*(1/24))</f>
+        <f t="shared" ref="G34" si="30">E34+(2*(1/24))</f>
         <v>0.70833333333333337</v>
       </c>
       <c r="H34" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" ref="H34:H38" si="31">VLOOKUP(A34,locations,2)</f>
         <v>Baku City Circuit</v>
       </c>
       <c r="I34" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" ref="I34:I38" si="32">VLOOKUP(A34,locations,3)</f>
         <v>Azerbaijan Grand Prix</v>
       </c>
     </row>
@@ -2001,7 +2006,7 @@
         <v>96</v>
       </c>
       <c r="C35" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>America/New_York</v>
       </c>
       <c r="D35" s="4">
@@ -2011,7 +2016,7 @@
         <v>0.5625</v>
       </c>
       <c r="F35" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>45051</v>
       </c>
       <c r="G35" s="5">
@@ -2019,11 +2024,11 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="H35" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>Miami International Autodrome</v>
       </c>
       <c r="I35" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>crypto.com Miami Grand Prix</v>
       </c>
     </row>
@@ -2035,7 +2040,7 @@
         <v>97</v>
       </c>
       <c r="C36" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>America/New_York</v>
       </c>
       <c r="D36" s="4">
@@ -2045,19 +2050,19 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F36" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>45051</v>
       </c>
       <c r="G36" s="5">
-        <f t="shared" ref="G36:G38" si="30">E36+(1/24)</f>
+        <f t="shared" ref="G36:G38" si="33">E36+(1/24)</f>
         <v>0.75</v>
       </c>
       <c r="H36" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>Miami International Autodrome</v>
       </c>
       <c r="I36" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>crypto.com Miami Grand Prix</v>
       </c>
     </row>
@@ -2069,7 +2074,7 @@
         <v>98</v>
       </c>
       <c r="C37" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>America/New_York</v>
       </c>
       <c r="D37" s="4">
@@ -2079,19 +2084,19 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="F37" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>45052</v>
       </c>
       <c r="G37" s="5">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0.5625</v>
       </c>
       <c r="H37" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>Miami International Autodrome</v>
       </c>
       <c r="I37" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>crypto.com Miami Grand Prix</v>
       </c>
     </row>
@@ -2103,7 +2108,7 @@
         <v>11</v>
       </c>
       <c r="C38" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>America/New_York</v>
       </c>
       <c r="D38" s="4">
@@ -2113,19 +2118,19 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="F38" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>45052</v>
       </c>
       <c r="G38" s="5">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>0.70833333333333326</v>
       </c>
       <c r="H38" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>Miami International Autodrome</v>
       </c>
       <c r="I38" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>crypto.com Miami Grand Prix</v>
       </c>
     </row>
@@ -2137,7 +2142,7 @@
         <v>10</v>
       </c>
       <c r="C39" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>America/New_York</v>
       </c>
       <c r="D39" s="4">
@@ -2147,19 +2152,19 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="F39" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>45053</v>
       </c>
       <c r="G39" s="5">
-        <f t="shared" ref="G39" si="31">E39+(2*(1/24))</f>
+        <f t="shared" ref="G39" si="34">E39+(2*(1/24))</f>
         <v>0.72916666666666674</v>
       </c>
       <c r="H39" t="str">
-        <f t="shared" ref="H39:H41" si="32">VLOOKUP(A39,locations,2)</f>
+        <f t="shared" ref="H39:H41" si="35">VLOOKUP(A39,locations,2)</f>
         <v>Miami International Autodrome</v>
       </c>
       <c r="I39" t="str">
-        <f t="shared" ref="I39:I41" si="33">VLOOKUP(A39,locations,3)</f>
+        <f t="shared" ref="I39:I41" si="36">VLOOKUP(A39,locations,3)</f>
         <v>crypto.com Miami Grand Prix</v>
       </c>
     </row>
@@ -2181,7 +2186,7 @@
         <v>0.5625</v>
       </c>
       <c r="F40" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>45065</v>
       </c>
       <c r="G40" s="5">
@@ -2189,11 +2194,11 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="H40" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>Autodromo Enzo e Dino Ferrari</v>
       </c>
       <c r="I40" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>Gran Premio del Made In Italy e dell'Emilia Romagna</v>
       </c>
     </row>
@@ -2215,19 +2220,19 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="F41" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>45065</v>
       </c>
       <c r="G41" s="5">
-        <f t="shared" ref="G41:G43" si="34">E41+(1/24)</f>
+        <f t="shared" ref="G41:G43" si="37">E41+(1/24)</f>
         <v>0.75</v>
       </c>
       <c r="H41" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>Autodromo Enzo e Dino Ferrari</v>
       </c>
       <c r="I41" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>Gran Premio del Made In Italy e dell'Emilia Romagna</v>
       </c>
     </row>
@@ -2253,7 +2258,7 @@
         <v>45066</v>
       </c>
       <c r="G42" s="5">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>0.5625</v>
       </c>
       <c r="H42" t="str">
@@ -2287,15 +2292,15 @@
         <v>45066</v>
       </c>
       <c r="G43" s="5">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>0.70833333333333326</v>
       </c>
       <c r="H43" t="str">
-        <f t="shared" ref="H43" si="35">VLOOKUP(A43,locations,2)</f>
+        <f t="shared" ref="H43" si="38">VLOOKUP(A43,locations,2)</f>
         <v>Autodromo Enzo e Dino Ferrari</v>
       </c>
       <c r="I43" t="str">
-        <f t="shared" ref="I43" si="36">VLOOKUP(A43,locations,3)</f>
+        <f t="shared" ref="I43" si="39">VLOOKUP(A43,locations,3)</f>
         <v>Gran Premio del Made In Italy e dell'Emilia Romagna</v>
       </c>
     </row>
@@ -2321,15 +2326,15 @@
         <v>45067</v>
       </c>
       <c r="G44" s="5">
-        <f t="shared" ref="G44" si="37">E44+(2*(1/24))</f>
+        <f t="shared" ref="G44" si="40">E44+(2*(1/24))</f>
         <v>0.70833333333333337</v>
       </c>
       <c r="H44" t="str">
-        <f t="shared" ref="H44:H47" si="38">VLOOKUP(A44,locations,2)</f>
+        <f t="shared" ref="H44:H47" si="41">VLOOKUP(A44,locations,2)</f>
         <v>Autodromo Enzo e Dino Ferrari</v>
       </c>
       <c r="I44" t="str">
-        <f t="shared" ref="I44:I47" si="39">VLOOKUP(A44,locations,3)</f>
+        <f t="shared" ref="I44:I47" si="42">VLOOKUP(A44,locations,3)</f>
         <v>Gran Premio del Made In Italy e dell'Emilia Romagna</v>
       </c>
     </row>
@@ -2359,11 +2364,11 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="H45" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>Circuit de Monaco</v>
       </c>
       <c r="I45" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>Grand Prix de Monaco</v>
       </c>
     </row>
@@ -2389,15 +2394,15 @@
         <v>45072</v>
       </c>
       <c r="G46" s="5">
-        <f t="shared" ref="G46:G48" si="40">E46+(1/24)</f>
+        <f t="shared" ref="G46:G48" si="43">E46+(1/24)</f>
         <v>0.75</v>
       </c>
       <c r="H46" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>Circuit de Monaco</v>
       </c>
       <c r="I46" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>Grand Prix de Monaco</v>
       </c>
     </row>
@@ -2423,15 +2428,15 @@
         <v>45073</v>
       </c>
       <c r="G47" s="5">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>0.5625</v>
       </c>
       <c r="H47" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>Circuit de Monaco</v>
       </c>
       <c r="I47" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>Grand Prix de Monaco</v>
       </c>
     </row>
@@ -2457,7 +2462,7 @@
         <v>45073</v>
       </c>
       <c r="G48" s="5">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>0.70833333333333326</v>
       </c>
       <c r="H48" t="str">
@@ -2491,15 +2496,15 @@
         <v>45074</v>
       </c>
       <c r="G49" s="5">
-        <f t="shared" ref="G49" si="41">E49+(2*(1/24))</f>
+        <f t="shared" ref="G49" si="44">E49+(2*(1/24))</f>
         <v>0.70833333333333337</v>
       </c>
       <c r="H49" t="str">
-        <f t="shared" ref="H49:H52" si="42">VLOOKUP(A49,locations,2)</f>
+        <f t="shared" ref="H49:H52" si="45">VLOOKUP(A49,locations,2)</f>
         <v>Circuit de Monaco</v>
       </c>
       <c r="I49" t="str">
-        <f t="shared" ref="I49:I52" si="43">VLOOKUP(A49,locations,3)</f>
+        <f t="shared" ref="I49:I52" si="46">VLOOKUP(A49,locations,3)</f>
         <v>Grand Prix de Monaco</v>
       </c>
     </row>
@@ -2529,11 +2534,11 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="H50" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>Circuit de Barcelona-Catalunya</v>
       </c>
       <c r="I50" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>Gran Premio de España</v>
       </c>
     </row>
@@ -2559,15 +2564,15 @@
         <v>45079</v>
       </c>
       <c r="G51" s="5">
-        <f t="shared" ref="G51:G53" si="44">E51+(1/24)</f>
+        <f t="shared" ref="G51:G53" si="47">E51+(1/24)</f>
         <v>0.75</v>
       </c>
       <c r="H51" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>Circuit de Barcelona-Catalunya</v>
       </c>
       <c r="I51" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>Gran Premio de España</v>
       </c>
     </row>
@@ -2593,15 +2598,15 @@
         <v>45080</v>
       </c>
       <c r="G52" s="5">
-        <f t="shared" si="44"/>
+        <f t="shared" si="47"/>
         <v>0.5625</v>
       </c>
       <c r="H52" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>Circuit de Barcelona-Catalunya</v>
       </c>
       <c r="I52" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>Gran Premio de España</v>
       </c>
     </row>
@@ -2627,7 +2632,7 @@
         <v>45080</v>
       </c>
       <c r="G53" s="5">
-        <f t="shared" si="44"/>
+        <f t="shared" si="47"/>
         <v>0.70833333333333326</v>
       </c>
       <c r="H53" t="str">
@@ -2661,15 +2666,15 @@
         <v>45081</v>
       </c>
       <c r="G54" s="5">
-        <f t="shared" ref="G54" si="45">E54+(2*(1/24))</f>
+        <f t="shared" ref="G54" si="48">E54+(2*(1/24))</f>
         <v>0.70833333333333337</v>
       </c>
       <c r="H54" t="str">
-        <f t="shared" ref="H54" si="46">VLOOKUP(A54,locations,2)</f>
+        <f t="shared" ref="H54" si="49">VLOOKUP(A54,locations,2)</f>
         <v>Circuit de Barcelona-Catalunya</v>
       </c>
       <c r="I54" t="str">
-        <f t="shared" ref="I54" si="47">VLOOKUP(A54,locations,3)</f>
+        <f t="shared" ref="I54" si="50">VLOOKUP(A54,locations,3)</f>
         <v>Gran Premio de España</v>
       </c>
     </row>
@@ -2699,11 +2704,11 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="H55" t="str">
-        <f t="shared" ref="H55:H64" si="48">VLOOKUP(A55,locations,2)</f>
+        <f t="shared" ref="H55:H64" si="51">VLOOKUP(A55,locations,2)</f>
         <v>Circuit Gilles-Villeneuve</v>
       </c>
       <c r="I55" t="str">
-        <f t="shared" ref="I55:I64" si="49">VLOOKUP(A55,locations,3)</f>
+        <f t="shared" ref="I55:I64" si="52">VLOOKUP(A55,locations,3)</f>
         <v>Grand Prix du Canada</v>
       </c>
     </row>
@@ -2729,15 +2734,15 @@
         <v>45093</v>
       </c>
       <c r="G56" s="5">
-        <f t="shared" ref="G56:G58" si="50">E56+(1/24)</f>
+        <f t="shared" ref="G56:G58" si="53">E56+(1/24)</f>
         <v>0.75</v>
       </c>
       <c r="H56" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>Circuit Gilles-Villeneuve</v>
       </c>
       <c r="I56" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>Grand Prix du Canada</v>
       </c>
     </row>
@@ -2763,15 +2768,15 @@
         <v>45094</v>
       </c>
       <c r="G57" s="5">
-        <f t="shared" si="50"/>
+        <f t="shared" si="53"/>
         <v>0.5625</v>
       </c>
       <c r="H57" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>Circuit Gilles-Villeneuve</v>
       </c>
       <c r="I57" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>Grand Prix du Canada</v>
       </c>
     </row>
@@ -2797,15 +2802,15 @@
         <v>45094</v>
       </c>
       <c r="G58" s="5">
-        <f t="shared" si="50"/>
+        <f t="shared" si="53"/>
         <v>0.70833333333333326</v>
       </c>
       <c r="H58" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>Circuit Gilles-Villeneuve</v>
       </c>
       <c r="I58" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>Grand Prix du Canada</v>
       </c>
     </row>
@@ -2831,15 +2836,15 @@
         <v>45095</v>
       </c>
       <c r="G59" s="5">
-        <f t="shared" ref="G59" si="51">E59+(2*(1/24))</f>
+        <f t="shared" ref="G59" si="54">E59+(2*(1/24))</f>
         <v>0.66666666666666674</v>
       </c>
       <c r="H59" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>Circuit Gilles-Villeneuve</v>
       </c>
       <c r="I59" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>Grand Prix du Canada</v>
       </c>
     </row>
@@ -2869,11 +2874,11 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="H60" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>Red Bull Ring</v>
       </c>
       <c r="I60" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>Grosser Preis von Österreich</v>
       </c>
     </row>
@@ -2899,15 +2904,15 @@
         <v>45107</v>
       </c>
       <c r="G61" s="5">
-        <f t="shared" ref="G61:G63" si="52">E61+(1/24)</f>
+        <f t="shared" ref="G61:G63" si="55">E61+(1/24)</f>
         <v>0.75</v>
       </c>
       <c r="H61" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>Red Bull Ring</v>
       </c>
       <c r="I61" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>Grosser Preis von Österreich</v>
       </c>
     </row>
@@ -2929,19 +2934,19 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="F62" s="4">
-        <f t="shared" ref="F62:F67" si="53">D62</f>
+        <f t="shared" ref="F62:F67" si="56">D62</f>
         <v>45108</v>
       </c>
       <c r="G62" s="5">
+        <f t="shared" si="55"/>
+        <v>0.5625</v>
+      </c>
+      <c r="H62" t="str">
+        <f t="shared" si="51"/>
+        <v>Red Bull Ring</v>
+      </c>
+      <c r="I62" t="str">
         <f t="shared" si="52"/>
-        <v>0.5625</v>
-      </c>
-      <c r="H62" t="str">
-        <f t="shared" si="48"/>
-        <v>Red Bull Ring</v>
-      </c>
-      <c r="I62" t="str">
-        <f t="shared" si="49"/>
         <v>Grosser Preis von Österreich</v>
       </c>
     </row>
@@ -2963,19 +2968,19 @@
         <v>0.6875</v>
       </c>
       <c r="F63" s="4">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>45108</v>
       </c>
       <c r="G63" s="5">
+        <f t="shared" si="55"/>
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="H63" t="str">
+        <f t="shared" si="51"/>
+        <v>Red Bull Ring</v>
+      </c>
+      <c r="I63" t="str">
         <f t="shared" si="52"/>
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="H63" t="str">
-        <f t="shared" si="48"/>
-        <v>Red Bull Ring</v>
-      </c>
-      <c r="I63" t="str">
-        <f t="shared" si="49"/>
         <v>Grosser Preis von Österreich</v>
       </c>
     </row>
@@ -2997,19 +3002,19 @@
         <v>0.625</v>
       </c>
       <c r="F64" s="4">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>45109</v>
       </c>
       <c r="G64" s="5">
-        <f t="shared" ref="G64" si="54">E64+(2*(1/24))</f>
+        <f t="shared" ref="G64" si="57">E64+(2*(1/24))</f>
         <v>0.70833333333333337</v>
       </c>
       <c r="H64" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>Red Bull Ring</v>
       </c>
       <c r="I64" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>Grosser Preis von Österreich</v>
       </c>
     </row>
@@ -3031,7 +3036,7 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="F65" s="4">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>45114</v>
       </c>
       <c r="G65" s="5">
@@ -3039,11 +3044,11 @@
         <v>0.5625</v>
       </c>
       <c r="H65" t="str">
-        <f t="shared" ref="H65:H84" si="55">VLOOKUP(A65,locations,2)</f>
+        <f t="shared" ref="H65:H84" si="58">VLOOKUP(A65,locations,2)</f>
         <v>Silverstone</v>
       </c>
       <c r="I65" t="str">
-        <f t="shared" ref="I65:I84" si="56">VLOOKUP(A65,locations,3)</f>
+        <f t="shared" ref="I65:I84" si="59">VLOOKUP(A65,locations,3)</f>
         <v>Aramco British Grand Prix</v>
       </c>
     </row>
@@ -3065,19 +3070,19 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="F66" s="4">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>45114</v>
       </c>
       <c r="G66" s="5">
-        <f t="shared" ref="G66:G68" si="57">E66+(1/24)</f>
+        <f t="shared" ref="G66:G68" si="60">E66+(1/24)</f>
         <v>0.70833333333333326</v>
       </c>
       <c r="H66" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>Silverstone</v>
       </c>
       <c r="I66" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>Aramco British Grand Prix</v>
       </c>
     </row>
@@ -3099,19 +3104,19 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="F67" s="4">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>45115</v>
       </c>
       <c r="G67" s="5">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>0.52083333333333337</v>
       </c>
       <c r="H67" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>Silverstone</v>
       </c>
       <c r="I67" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>Aramco British Grand Prix</v>
       </c>
     </row>
@@ -3137,15 +3142,15 @@
         <v>45115</v>
       </c>
       <c r="G68" s="5">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="H68" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>Silverstone</v>
       </c>
       <c r="I68" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>Aramco British Grand Prix</v>
       </c>
     </row>
@@ -3171,15 +3176,15 @@
         <v>45116</v>
       </c>
       <c r="G69" s="5">
-        <f t="shared" ref="G69" si="58">E69+(2*(1/24))</f>
+        <f t="shared" ref="G69" si="61">E69+(2*(1/24))</f>
         <v>0.70833333333333337</v>
       </c>
       <c r="H69" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>Silverstone</v>
       </c>
       <c r="I69" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>Aramco British Grand Prix</v>
       </c>
     </row>
@@ -3209,11 +3214,11 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="H70" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>Hungaroring</v>
       </c>
       <c r="I70" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>Magyar Nagydíj</v>
       </c>
     </row>
@@ -3239,15 +3244,15 @@
         <v>45128</v>
       </c>
       <c r="G71" s="5">
-        <f t="shared" ref="G71:G73" si="59">E71+(1/24)</f>
+        <f t="shared" ref="G71:G73" si="62">E71+(1/24)</f>
         <v>0.75</v>
       </c>
       <c r="H71" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>Hungaroring</v>
       </c>
       <c r="I71" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>Magyar Nagydíj</v>
       </c>
     </row>
@@ -3273,15 +3278,15 @@
         <v>45129</v>
       </c>
       <c r="G72" s="5">
+        <f t="shared" si="62"/>
+        <v>0.5625</v>
+      </c>
+      <c r="H72" t="str">
+        <f t="shared" si="58"/>
+        <v>Hungaroring</v>
+      </c>
+      <c r="I72" t="str">
         <f t="shared" si="59"/>
-        <v>0.5625</v>
-      </c>
-      <c r="H72" t="str">
-        <f t="shared" si="55"/>
-        <v>Hungaroring</v>
-      </c>
-      <c r="I72" t="str">
-        <f t="shared" si="56"/>
         <v>Magyar Nagydíj</v>
       </c>
     </row>
@@ -3307,15 +3312,15 @@
         <v>45129</v>
       </c>
       <c r="G73" s="5">
+        <f t="shared" si="62"/>
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="H73" t="str">
+        <f t="shared" si="58"/>
+        <v>Hungaroring</v>
+      </c>
+      <c r="I73" t="str">
         <f t="shared" si="59"/>
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="H73" t="str">
-        <f t="shared" si="55"/>
-        <v>Hungaroring</v>
-      </c>
-      <c r="I73" t="str">
-        <f t="shared" si="56"/>
         <v>Magyar Nagydíj</v>
       </c>
     </row>
@@ -3341,15 +3346,15 @@
         <v>45130</v>
       </c>
       <c r="G74" s="5">
-        <f t="shared" ref="G74" si="60">E74+(2*(1/24))</f>
+        <f t="shared" ref="G74" si="63">E74+(2*(1/24))</f>
         <v>0.70833333333333337</v>
       </c>
       <c r="H74" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>Hungaroring</v>
       </c>
       <c r="I74" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>Magyar Nagydíj</v>
       </c>
     </row>
@@ -3379,11 +3384,11 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="H75" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>Circuit de Spa-Francorchamps</v>
       </c>
       <c r="I75" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>Belgian Grand Prix</v>
       </c>
     </row>
@@ -3409,15 +3414,15 @@
         <v>45135</v>
       </c>
       <c r="G76" s="5">
-        <f t="shared" ref="G76:G78" si="61">E76+(1/24)</f>
+        <f t="shared" ref="G76:G78" si="64">E76+(1/24)</f>
         <v>0.75</v>
       </c>
       <c r="H76" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>Circuit de Spa-Francorchamps</v>
       </c>
       <c r="I76" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>Belgian Grand Prix</v>
       </c>
     </row>
@@ -3443,15 +3448,15 @@
         <v>45136</v>
       </c>
       <c r="G77" s="5">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>0.5625</v>
       </c>
       <c r="H77" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>Circuit de Spa-Francorchamps</v>
       </c>
       <c r="I77" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>Belgian Grand Prix</v>
       </c>
     </row>
@@ -3477,15 +3482,15 @@
         <v>45136</v>
       </c>
       <c r="G78" s="5">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>0.72916666666666663</v>
       </c>
       <c r="H78" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>Circuit de Spa-Francorchamps</v>
       </c>
       <c r="I78" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>Belgian Grand Prix</v>
       </c>
     </row>
@@ -3511,15 +3516,15 @@
         <v>45137</v>
       </c>
       <c r="G79" s="5">
-        <f t="shared" ref="G79" si="62">E79+(2*(1/24))</f>
+        <f t="shared" ref="G79" si="65">E79+(2*(1/24))</f>
         <v>0.70833333333333337</v>
       </c>
       <c r="H79" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>Circuit de Spa-Francorchamps</v>
       </c>
       <c r="I79" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>Belgian Grand Prix</v>
       </c>
     </row>
@@ -3549,11 +3554,11 @@
         <v>0.5625</v>
       </c>
       <c r="H80" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>Circuit Zandvoort</v>
       </c>
       <c r="I80" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>Heineken Dutch Grand Prix</v>
       </c>
     </row>
@@ -3579,15 +3584,15 @@
         <v>45163</v>
       </c>
       <c r="G81" s="5">
-        <f t="shared" ref="G81:G83" si="63">E81+(1/24)</f>
+        <f t="shared" ref="G81:G83" si="66">E81+(1/24)</f>
         <v>0.70833333333333326</v>
       </c>
       <c r="H81" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>Circuit Zandvoort</v>
       </c>
       <c r="I81" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>Heineken Dutch Grand Prix</v>
       </c>
     </row>
@@ -3613,15 +3618,15 @@
         <v>45164</v>
       </c>
       <c r="G82" s="5">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>0.52083333333333337</v>
       </c>
       <c r="H82" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>Circuit Zandvoort</v>
       </c>
       <c r="I82" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>Heineken Dutch Grand Prix</v>
       </c>
     </row>
@@ -3647,15 +3652,15 @@
         <v>45164</v>
       </c>
       <c r="G83" s="5">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="H83" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>Circuit Zandvoort</v>
       </c>
       <c r="I83" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>Heineken Dutch Grand Prix</v>
       </c>
     </row>
@@ -3681,15 +3686,15 @@
         <v>45165</v>
       </c>
       <c r="G84" s="5">
-        <f t="shared" ref="G84" si="64">E84+(2*(1/24))</f>
+        <f t="shared" ref="G84" si="67">E84+(2*(1/24))</f>
         <v>0.70833333333333337</v>
       </c>
       <c r="H84" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>Circuit Zandvoort</v>
       </c>
       <c r="I84" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>Heineken Dutch Grand Prix</v>
       </c>
     </row>
@@ -3719,11 +3724,11 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="H85" t="str">
-        <f t="shared" ref="H85:H99" si="65">VLOOKUP(A85,locations,2)</f>
+        <f t="shared" ref="H85:H99" si="68">VLOOKUP(A85,locations,2)</f>
         <v>Autodromo Nazionale Monza</v>
       </c>
       <c r="I85" t="str">
-        <f t="shared" ref="I85:I99" si="66">VLOOKUP(A85,locations,3)</f>
+        <f t="shared" ref="I85:I99" si="69">VLOOKUP(A85,locations,3)</f>
         <v>Gran Premio d'Italia</v>
       </c>
     </row>
@@ -3749,15 +3754,15 @@
         <v>45170</v>
       </c>
       <c r="G86" s="5">
-        <f t="shared" ref="G86:G88" si="67">E86+(1/24)</f>
+        <f t="shared" ref="G86:G88" si="70">E86+(1/24)</f>
         <v>0.75</v>
       </c>
       <c r="H86" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>Autodromo Nazionale Monza</v>
       </c>
       <c r="I86" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="69"/>
         <v>Gran Premio d'Italia</v>
       </c>
     </row>
@@ -3783,15 +3788,15 @@
         <v>45171</v>
       </c>
       <c r="G87" s="5">
-        <f t="shared" si="67"/>
+        <f t="shared" si="70"/>
         <v>0.5625</v>
       </c>
       <c r="H87" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>Autodromo Nazionale Monza</v>
       </c>
       <c r="I87" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="69"/>
         <v>Gran Premio d'Italia</v>
       </c>
     </row>
@@ -3817,15 +3822,15 @@
         <v>45171</v>
       </c>
       <c r="G88" s="5">
-        <f t="shared" si="67"/>
+        <f t="shared" si="70"/>
         <v>0.70833333333333326</v>
       </c>
       <c r="H88" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>Autodromo Nazionale Monza</v>
       </c>
       <c r="I88" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="69"/>
         <v>Gran Premio d'Italia</v>
       </c>
     </row>
@@ -3851,15 +3856,15 @@
         <v>45172</v>
       </c>
       <c r="G89" s="5">
-        <f t="shared" ref="G89" si="68">E89+(2*(1/24))</f>
+        <f t="shared" ref="G89" si="71">E89+(2*(1/24))</f>
         <v>0.70833333333333337</v>
       </c>
       <c r="H89" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>Autodromo Nazionale Monza</v>
       </c>
       <c r="I89" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="69"/>
         <v>Gran Premio d'Italia</v>
       </c>
     </row>
@@ -3889,11 +3894,11 @@
         <v>0.77083333333333326</v>
       </c>
       <c r="H90" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>Marina Bay Street Circuit</v>
       </c>
       <c r="I90" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="69"/>
         <v>Singapore Airlines Singapore Grand Prix</v>
       </c>
     </row>
@@ -3919,15 +3924,15 @@
         <v>45184</v>
       </c>
       <c r="G91" s="5">
-        <f t="shared" ref="G91:G93" si="69">E91+(1/24)</f>
+        <f t="shared" ref="G91:G93" si="72">E91+(1/24)</f>
         <v>0.91666666666666663</v>
       </c>
       <c r="H91" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>Marina Bay Street Circuit</v>
       </c>
       <c r="I91" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="69"/>
         <v>Singapore Airlines Singapore Grand Prix</v>
       </c>
     </row>
@@ -3953,15 +3958,15 @@
         <v>45185</v>
       </c>
       <c r="G92" s="5">
+        <f t="shared" si="72"/>
+        <v>0.77083333333333326</v>
+      </c>
+      <c r="H92" t="str">
+        <f t="shared" si="68"/>
+        <v>Marina Bay Street Circuit</v>
+      </c>
+      <c r="I92" t="str">
         <f t="shared" si="69"/>
-        <v>0.77083333333333326</v>
-      </c>
-      <c r="H92" t="str">
-        <f t="shared" si="65"/>
-        <v>Marina Bay Street Circuit</v>
-      </c>
-      <c r="I92" t="str">
-        <f t="shared" si="66"/>
         <v>Singapore Airlines Singapore Grand Prix</v>
       </c>
     </row>
@@ -3987,15 +3992,15 @@
         <v>45185</v>
       </c>
       <c r="G93" s="5">
+        <f t="shared" si="72"/>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="H93" t="str">
+        <f t="shared" si="68"/>
+        <v>Marina Bay Street Circuit</v>
+      </c>
+      <c r="I93" t="str">
         <f t="shared" si="69"/>
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="H93" t="str">
-        <f t="shared" si="65"/>
-        <v>Marina Bay Street Circuit</v>
-      </c>
-      <c r="I93" t="str">
-        <f t="shared" si="66"/>
         <v>Singapore Airlines Singapore Grand Prix</v>
       </c>
     </row>
@@ -4021,15 +4026,15 @@
         <v>45186</v>
       </c>
       <c r="G94" s="5">
-        <f t="shared" ref="G94" si="70">E94+(2*(1/24))</f>
+        <f t="shared" ref="G94" si="73">E94+(2*(1/24))</f>
         <v>0.91666666666666674</v>
       </c>
       <c r="H94" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>Marina Bay Street Circuit</v>
       </c>
       <c r="I94" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="69"/>
         <v>Singapore Airlines Singapore Grand Prix</v>
       </c>
     </row>
@@ -4059,11 +4064,11 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="H95" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>Suzuka International Racing Course</v>
       </c>
       <c r="I95" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="69"/>
         <v>Lenovo Japanese Grand Prix</v>
       </c>
     </row>
@@ -4089,15 +4094,15 @@
         <v>45191</v>
       </c>
       <c r="G96" s="5">
-        <f t="shared" ref="G96:G98" si="71">E96+(1/24)</f>
+        <f t="shared" ref="G96:G98" si="74">E96+(1/24)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="H96" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>Suzuka International Racing Course</v>
       </c>
       <c r="I96" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="69"/>
         <v>Lenovo Japanese Grand Prix</v>
       </c>
     </row>
@@ -4123,15 +4128,15 @@
         <v>45192</v>
       </c>
       <c r="G97" s="5">
-        <f t="shared" si="71"/>
+        <f t="shared" si="74"/>
         <v>0.52083333333333337</v>
       </c>
       <c r="H97" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>Suzuka International Racing Course</v>
       </c>
       <c r="I97" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="69"/>
         <v>Lenovo Japanese Grand Prix</v>
       </c>
     </row>
@@ -4157,15 +4162,15 @@
         <v>45192</v>
       </c>
       <c r="G98" s="5">
-        <f t="shared" si="71"/>
+        <f t="shared" si="74"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="H98" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>Suzuka International Racing Course</v>
       </c>
       <c r="I98" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="69"/>
         <v>Lenovo Japanese Grand Prix</v>
       </c>
     </row>
@@ -4191,15 +4196,15 @@
         <v>45193</v>
       </c>
       <c r="G99" s="5">
-        <f t="shared" ref="G99" si="72">E99+(2*(1/24))</f>
+        <f t="shared" ref="G99" si="75">E99+(2*(1/24))</f>
         <v>0.66666666666666674</v>
       </c>
       <c r="H99" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>Suzuka International Racing Course</v>
       </c>
       <c r="I99" t="str">
-        <f t="shared" si="66"/>
+        <f t="shared" si="69"/>
         <v>Lenovo Japanese Grand Prix</v>
       </c>
     </row>
@@ -4229,11 +4234,11 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="H100" t="str">
-        <f t="shared" ref="H100:H109" si="73">VLOOKUP(A100,locations,2)</f>
+        <f t="shared" ref="H100:H109" si="76">VLOOKUP(A100,locations,2)</f>
         <v>Lusail International Circuit</v>
       </c>
       <c r="I100" t="str">
-        <f t="shared" ref="I100:I109" si="74">VLOOKUP(A100,locations,3)</f>
+        <f t="shared" ref="I100:I109" si="77">VLOOKUP(A100,locations,3)</f>
         <v>Qatar Grand Prix</v>
       </c>
     </row>
@@ -4259,15 +4264,15 @@
         <v>45205</v>
       </c>
       <c r="G101" s="5">
-        <f t="shared" ref="G101:G103" si="75">E101+(1/24)</f>
+        <f t="shared" ref="G101:G103" si="78">E101+(1/24)</f>
         <v>0.75</v>
       </c>
       <c r="H101" t="str">
-        <f t="shared" si="73"/>
+        <f t="shared" si="76"/>
         <v>Lusail International Circuit</v>
       </c>
       <c r="I101" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="77"/>
         <v>Qatar Grand Prix</v>
       </c>
     </row>
@@ -4293,15 +4298,15 @@
         <v>45206</v>
       </c>
       <c r="G102" s="5">
-        <f t="shared" si="75"/>
+        <f t="shared" si="78"/>
         <v>0.60416666666666663</v>
       </c>
       <c r="H102" t="str">
-        <f t="shared" si="73"/>
+        <f t="shared" si="76"/>
         <v>Lusail International Circuit</v>
       </c>
       <c r="I102" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="77"/>
         <v>Qatar Grand Prix</v>
       </c>
     </row>
@@ -4327,15 +4332,15 @@
         <v>45206</v>
       </c>
       <c r="G103" s="5">
-        <f t="shared" si="75"/>
+        <f t="shared" si="78"/>
         <v>0.77083333333333326</v>
       </c>
       <c r="H103" t="str">
-        <f t="shared" si="73"/>
+        <f t="shared" si="76"/>
         <v>Lusail International Circuit</v>
       </c>
       <c r="I103" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="77"/>
         <v>Qatar Grand Prix</v>
       </c>
     </row>
@@ -4361,15 +4366,15 @@
         <v>45207</v>
       </c>
       <c r="G104" s="5">
-        <f t="shared" ref="G104" si="76">E104+(2*(1/24))</f>
+        <f t="shared" ref="G104" si="79">E104+(2*(1/24))</f>
         <v>0.79166666666666674</v>
       </c>
       <c r="H104" t="str">
-        <f t="shared" si="73"/>
+        <f t="shared" si="76"/>
         <v>Lusail International Circuit</v>
       </c>
       <c r="I104" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="77"/>
         <v>Qatar Grand Prix</v>
       </c>
     </row>
@@ -4399,11 +4404,11 @@
         <v>0.5625</v>
       </c>
       <c r="H105" t="str">
-        <f t="shared" si="73"/>
+        <f t="shared" si="76"/>
         <v>Circuit of The Americas</v>
       </c>
       <c r="I105" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="77"/>
         <v>Lenovo United States Grand Prix</v>
       </c>
     </row>
@@ -4429,15 +4434,15 @@
         <v>45219</v>
       </c>
       <c r="G106" s="5">
-        <f t="shared" ref="G106:G108" si="77">E106+(1/24)</f>
+        <f t="shared" ref="G106:G108" si="80">E106+(1/24)</f>
         <v>0.70833333333333326</v>
       </c>
       <c r="H106" t="str">
-        <f t="shared" si="73"/>
+        <f t="shared" si="76"/>
         <v>Circuit of The Americas</v>
       </c>
       <c r="I106" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="77"/>
         <v>Lenovo United States Grand Prix</v>
       </c>
     </row>
@@ -4463,15 +4468,15 @@
         <v>45220</v>
       </c>
       <c r="G107" s="5">
+        <f t="shared" si="80"/>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="H107" t="str">
+        <f t="shared" si="76"/>
+        <v>Circuit of The Americas</v>
+      </c>
+      <c r="I107" t="str">
         <f t="shared" si="77"/>
-        <v>0.58333333333333326</v>
-      </c>
-      <c r="H107" t="str">
-        <f t="shared" si="73"/>
-        <v>Circuit of The Americas</v>
-      </c>
-      <c r="I107" t="str">
-        <f t="shared" si="74"/>
         <v>Lenovo United States Grand Prix</v>
       </c>
     </row>
@@ -4497,15 +4502,15 @@
         <v>45220</v>
       </c>
       <c r="G108" s="5">
+        <f t="shared" si="80"/>
+        <v>0.75</v>
+      </c>
+      <c r="H108" t="str">
+        <f t="shared" si="76"/>
+        <v>Circuit of The Americas</v>
+      </c>
+      <c r="I108" t="str">
         <f t="shared" si="77"/>
-        <v>0.75</v>
-      </c>
-      <c r="H108" t="str">
-        <f t="shared" si="73"/>
-        <v>Circuit of The Americas</v>
-      </c>
-      <c r="I108" t="str">
-        <f t="shared" si="74"/>
         <v>Lenovo United States Grand Prix</v>
       </c>
     </row>
@@ -4531,15 +4536,15 @@
         <v>45221</v>
       </c>
       <c r="G109" s="5">
-        <f t="shared" ref="G109" si="78">E109+(2*(1/24))</f>
+        <f t="shared" ref="G109" si="81">E109+(2*(1/24))</f>
         <v>0.66666666666666674</v>
       </c>
       <c r="H109" t="str">
-        <f t="shared" si="73"/>
+        <f t="shared" si="76"/>
         <v>Circuit of The Americas</v>
       </c>
       <c r="I109" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="77"/>
         <v>Lenovo United States Grand Prix</v>
       </c>
     </row>
@@ -4569,11 +4574,11 @@
         <v>0.5625</v>
       </c>
       <c r="H110" t="str">
-        <f t="shared" ref="H110:H114" si="79">VLOOKUP(A110,locations,2)</f>
+        <f t="shared" ref="H110:H114" si="82">VLOOKUP(A110,locations,2)</f>
         <v>Autódromo Hermanos Rodríguez</v>
       </c>
       <c r="I110" t="str">
-        <f t="shared" ref="I110:I114" si="80">VLOOKUP(A110,locations,3)</f>
+        <f t="shared" ref="I110:I114" si="83">VLOOKUP(A110,locations,3)</f>
         <v>Gran Premio de la Ciudad de México</v>
       </c>
     </row>
@@ -4599,15 +4604,15 @@
         <v>45226</v>
       </c>
       <c r="G111" s="5">
-        <f t="shared" ref="G111:G113" si="81">E111+(1/24)</f>
+        <f t="shared" ref="G111:G113" si="84">E111+(1/24)</f>
         <v>0.70833333333333326</v>
       </c>
       <c r="H111" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" si="82"/>
         <v>Autódromo Hermanos Rodríguez</v>
       </c>
       <c r="I111" t="str">
-        <f t="shared" si="80"/>
+        <f t="shared" si="83"/>
         <v>Gran Premio de la Ciudad de México</v>
       </c>
     </row>
@@ -4633,15 +4638,15 @@
         <v>45227</v>
       </c>
       <c r="G112" s="5">
-        <f t="shared" si="81"/>
+        <f t="shared" si="84"/>
         <v>0.52083333333333337</v>
       </c>
       <c r="H112" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" si="82"/>
         <v>Autódromo Hermanos Rodríguez</v>
       </c>
       <c r="I112" t="str">
-        <f t="shared" si="80"/>
+        <f t="shared" si="83"/>
         <v>Gran Premio de la Ciudad de México</v>
       </c>
     </row>
@@ -4667,15 +4672,15 @@
         <v>45227</v>
       </c>
       <c r="G113" s="5">
-        <f t="shared" si="81"/>
+        <f t="shared" si="84"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="H113" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" si="82"/>
         <v>Autódromo Hermanos Rodríguez</v>
       </c>
       <c r="I113" t="str">
-        <f t="shared" si="80"/>
+        <f t="shared" si="83"/>
         <v>Gran Premio de la Ciudad de México</v>
       </c>
     </row>
@@ -4701,15 +4706,15 @@
         <v>45228</v>
       </c>
       <c r="G114" s="5">
-        <f t="shared" ref="G114" si="82">E114+(2*(1/24))</f>
+        <f t="shared" ref="G114" si="85">E114+(2*(1/24))</f>
         <v>0.66666666666666674</v>
       </c>
       <c r="H114" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" si="82"/>
         <v>Autódromo Hermanos Rodríguez</v>
       </c>
       <c r="I114" t="str">
-        <f t="shared" si="80"/>
+        <f t="shared" si="83"/>
         <v>Gran Premio de la Ciudad de México</v>
       </c>
     </row>
@@ -4739,11 +4744,11 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="H115" t="str">
-        <f t="shared" ref="H115:H119" si="83">VLOOKUP(A115,locations,2)</f>
+        <f t="shared" ref="H115:H119" si="86">VLOOKUP(A115,locations,2)</f>
         <v>Autódromo José Carlos Pace</v>
       </c>
       <c r="I115" t="str">
-        <f t="shared" ref="I115:I119" si="84">VLOOKUP(A115,locations,3)</f>
+        <f t="shared" ref="I115:I119" si="87">VLOOKUP(A115,locations,3)</f>
         <v>Rolex Grande Prêmio de São Paulo</v>
       </c>
     </row>
@@ -4769,15 +4774,15 @@
         <v>45233</v>
       </c>
       <c r="G116" s="5">
-        <f t="shared" ref="G116:G118" si="85">E116+(1/24)</f>
+        <f t="shared" ref="G116:G118" si="88">E116+(1/24)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="H116" t="str">
-        <f t="shared" si="83"/>
+        <f t="shared" si="86"/>
         <v>Autódromo José Carlos Pace</v>
       </c>
       <c r="I116" t="str">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>Rolex Grande Prêmio de São Paulo</v>
       </c>
     </row>
@@ -4803,15 +4808,15 @@
         <v>45234</v>
       </c>
       <c r="G117" s="5">
-        <f t="shared" si="85"/>
+        <f t="shared" si="88"/>
         <v>0.52083333333333337</v>
       </c>
       <c r="H117" t="str">
-        <f t="shared" si="83"/>
+        <f t="shared" si="86"/>
         <v>Autódromo José Carlos Pace</v>
       </c>
       <c r="I117" t="str">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>Rolex Grande Prêmio de São Paulo</v>
       </c>
     </row>
@@ -4837,15 +4842,15 @@
         <v>45234</v>
       </c>
       <c r="G118" s="5">
-        <f t="shared" si="85"/>
+        <f t="shared" si="88"/>
         <v>0.6875</v>
       </c>
       <c r="H118" t="str">
-        <f t="shared" si="83"/>
+        <f t="shared" si="86"/>
         <v>Autódromo José Carlos Pace</v>
       </c>
       <c r="I118" t="str">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>Rolex Grande Prêmio de São Paulo</v>
       </c>
     </row>
@@ -4871,15 +4876,15 @@
         <v>45235</v>
       </c>
       <c r="G119" s="5">
-        <f t="shared" ref="G119" si="86">E119+(2*(1/24))</f>
+        <f t="shared" ref="G119" si="89">E119+(2*(1/24))</f>
         <v>0.66666666666666674</v>
       </c>
       <c r="H119" t="str">
-        <f t="shared" si="83"/>
+        <f t="shared" si="86"/>
         <v>Autódromo José Carlos Pace</v>
       </c>
       <c r="I119" t="str">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>Rolex Grande Prêmio de São Paulo</v>
       </c>
     </row>
@@ -4909,11 +4914,11 @@
         <v>0.8125</v>
       </c>
       <c r="H120" t="str">
-        <f t="shared" ref="H120:H124" si="87">VLOOKUP(A120,locations,2)</f>
+        <f t="shared" ref="H120:H124" si="90">VLOOKUP(A120,locations,2)</f>
         <v>Las Vegas</v>
       </c>
       <c r="I120" t="str">
-        <f t="shared" ref="I120:I124" si="88">VLOOKUP(A120,locations,3)</f>
+        <f t="shared" ref="I120:I124" si="91">VLOOKUP(A120,locations,3)</f>
         <v>Heineken Silver Las Vegas Grand Prix</v>
       </c>
     </row>
@@ -4939,15 +4944,15 @@
         <v>45246</v>
       </c>
       <c r="G121" s="5">
-        <f t="shared" ref="G121:G123" si="89">E121+(1/24)</f>
+        <f t="shared" ref="G121:G123" si="92">E121+(1/24)</f>
         <v>0.95833333333333326</v>
       </c>
       <c r="H121" t="str">
-        <f t="shared" si="87"/>
+        <f t="shared" si="90"/>
         <v>Las Vegas</v>
       </c>
       <c r="I121" t="str">
-        <f t="shared" si="88"/>
+        <f t="shared" si="91"/>
         <v>Heineken Silver Las Vegas Grand Prix</v>
       </c>
     </row>
@@ -4973,15 +4978,15 @@
         <v>45247</v>
       </c>
       <c r="G122" s="5">
-        <f t="shared" si="89"/>
+        <f t="shared" si="92"/>
         <v>0.8125</v>
       </c>
       <c r="H122" t="str">
-        <f t="shared" si="87"/>
+        <f t="shared" si="90"/>
         <v>Las Vegas</v>
       </c>
       <c r="I122" t="str">
-        <f t="shared" si="88"/>
+        <f t="shared" si="91"/>
         <v>Heineken Silver Las Vegas Grand Prix</v>
       </c>
     </row>
@@ -5007,15 +5012,15 @@
         <v>45247</v>
       </c>
       <c r="G123" s="5">
-        <f t="shared" si="89"/>
+        <f t="shared" si="92"/>
         <v>0.95833333333333326</v>
       </c>
       <c r="H123" t="str">
-        <f t="shared" si="87"/>
+        <f t="shared" si="90"/>
         <v>Las Vegas</v>
       </c>
       <c r="I123" t="str">
-        <f t="shared" si="88"/>
+        <f t="shared" si="91"/>
         <v>Heineken Silver Las Vegas Grand Prix</v>
       </c>
     </row>
@@ -5040,15 +5045,15 @@
         <v>45249</v>
       </c>
       <c r="G124" s="5">
-        <f t="shared" ref="G124" si="90">E124+(2*(1/24))</f>
+        <f t="shared" ref="G124" si="93">E124+(2*(1/24))</f>
         <v>1</v>
       </c>
       <c r="H124" t="str">
-        <f t="shared" si="87"/>
+        <f t="shared" si="90"/>
         <v>Las Vegas</v>
       </c>
       <c r="I124" t="str">
-        <f t="shared" si="88"/>
+        <f t="shared" si="91"/>
         <v>Heineken Silver Las Vegas Grand Prix</v>
       </c>
     </row>
@@ -5078,11 +5083,11 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="H125" t="str">
-        <f t="shared" ref="H125:H127" si="91">VLOOKUP(A125,locations,2)</f>
+        <f t="shared" ref="H125:H127" si="94">VLOOKUP(A125,locations,2)</f>
         <v>Yas Marina Circuit</v>
       </c>
       <c r="I125" t="str">
-        <f t="shared" ref="I125:I127" si="92">VLOOKUP(A125,locations,3)</f>
+        <f t="shared" ref="I125:I127" si="95">VLOOKUP(A125,locations,3)</f>
         <v>Etihad Airways Abu Dhabi Grand Prix</v>
       </c>
     </row>
@@ -5108,15 +5113,15 @@
         <v>45254</v>
       </c>
       <c r="G126" s="5">
-        <f t="shared" ref="G126:G128" si="93">E126+(1/24)</f>
+        <f t="shared" ref="G126:G128" si="96">E126+(1/24)</f>
         <v>0.75</v>
       </c>
       <c r="H126" t="str">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>Yas Marina Circuit</v>
       </c>
       <c r="I126" t="str">
-        <f t="shared" si="92"/>
+        <f t="shared" si="95"/>
         <v>Etihad Airways Abu Dhabi Grand Prix</v>
       </c>
     </row>
@@ -5142,15 +5147,15 @@
         <v>45255</v>
       </c>
       <c r="G127" s="5">
-        <f t="shared" si="93"/>
+        <f t="shared" si="96"/>
         <v>0.64583333333333326</v>
       </c>
       <c r="H127" t="str">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>Yas Marina Circuit</v>
       </c>
       <c r="I127" t="str">
-        <f t="shared" si="92"/>
+        <f t="shared" si="95"/>
         <v>Etihad Airways Abu Dhabi Grand Prix</v>
       </c>
     </row>
@@ -5176,7 +5181,7 @@
         <v>45255</v>
       </c>
       <c r="G128" s="5">
-        <f t="shared" si="93"/>
+        <f t="shared" si="96"/>
         <v>0.79166666666666663</v>
       </c>
       <c r="H128" t="str">
@@ -5210,15 +5215,15 @@
         <v>45256</v>
       </c>
       <c r="G129" s="5">
-        <f t="shared" ref="G129" si="94">E129+(2*(1/24))</f>
+        <f t="shared" ref="G129" si="97">E129+(2*(1/24))</f>
         <v>0.79166666666666674</v>
       </c>
       <c r="H129" t="str">
-        <f t="shared" ref="H129" si="95">VLOOKUP(A129,locations,2)</f>
+        <f t="shared" ref="H129" si="98">VLOOKUP(A129,locations,2)</f>
         <v>Yas Marina Circuit</v>
       </c>
       <c r="I129" t="str">
-        <f t="shared" ref="I129" si="96">VLOOKUP(A129,locations,3)</f>
+        <f t="shared" ref="I129" si="99">VLOOKUP(A129,locations,3)</f>
         <v>Etihad Airways Abu Dhabi Grand Prix</v>
       </c>
     </row>
@@ -5252,7 +5257,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:I11"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5261,6 +5266,7 @@
     <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="44.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -5348,7 +5354,7 @@
         <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>141</v>
       </c>
       <c r="H4" t="s">
         <v>119</v>
@@ -5371,7 +5377,7 @@
         <v>82</v>
       </c>
       <c r="F5" t="s">
-        <v>98</v>
+        <v>11</v>
       </c>
       <c r="H5" t="s">
         <v>92</v>
@@ -5394,7 +5400,7 @@
         <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H6" t="s">
         <v>93</v>
@@ -5417,7 +5423,7 @@
         <v>81</v>
       </c>
       <c r="F7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H7" t="s">
         <v>137</v>
@@ -5440,7 +5446,7 @@
         <v>94</v>
       </c>
       <c r="F8" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="H8" t="s">
         <v>125</v>
@@ -5463,7 +5469,7 @@
         <v>95</v>
       </c>
       <c r="F9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H9" t="s">
         <v>122</v>
@@ -5484,6 +5490,9 @@
       </c>
       <c r="D10" t="s">
         <v>32</v>
+      </c>
+      <c r="F10" t="s">
+        <v>91</v>
       </c>
       <c r="H10" t="s">
         <v>138</v>

</xml_diff>

<commit_message>
Add Sprint Shootout details
</commit_message>
<xml_diff>
--- a/f1/F1.xlsx
+++ b/f1/F1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin/projects/calendars/f1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B6932B8-A661-7443-9DF9-F8535BAE0728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{03DB6C78-D5CE-A245-BFB5-AA900B61CD3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3440" yWindow="780" windowWidth="28040" windowHeight="17440" xr2:uid="{65D0735D-D923-6F47-A559-767DB601EBAB}"/>
   </bookViews>
@@ -950,7 +950,7 @@
   <dimension ref="A1:I129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="G118" sqref="G118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2921,7 +2921,7 @@
         <v>18</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>97</v>
+        <v>141</v>
       </c>
       <c r="C62" t="str">
         <f>VLOOKUP(A62,locations,4)</f>
@@ -2931,15 +2931,15 @@
         <v>45108</v>
       </c>
       <c r="E62" s="5">
-        <v>0.52083333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="F62" s="4">
         <f t="shared" ref="F62:F67" si="56">D62</f>
         <v>45108</v>
       </c>
       <c r="G62" s="5">
-        <f t="shared" si="55"/>
-        <v>0.5625</v>
+        <f>E62+(3*(1/96))</f>
+        <v>0.53125</v>
       </c>
       <c r="H62" t="str">
         <f t="shared" si="51"/>
@@ -3431,7 +3431,7 @@
         <v>57</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>97</v>
+        <v>141</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="1"/>
@@ -3441,15 +3441,15 @@
         <v>45136</v>
       </c>
       <c r="E77" s="5">
-        <v>0.52083333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="F77" s="4">
         <f t="shared" si="15"/>
         <v>45136</v>
       </c>
       <c r="G77" s="5">
-        <f t="shared" si="64"/>
-        <v>0.5625</v>
+        <f>E77+(3*(1/96))</f>
+        <v>0.53125</v>
       </c>
       <c r="H77" t="str">
         <f t="shared" si="58"/>
@@ -4223,7 +4223,7 @@
         <v>45205</v>
       </c>
       <c r="E100" s="7">
-        <v>0.5625</v>
+        <v>0.6875</v>
       </c>
       <c r="F100" s="4">
         <f t="shared" si="15"/>
@@ -4231,7 +4231,7 @@
       </c>
       <c r="G100" s="5">
         <f>E100+(1/24)</f>
-        <v>0.60416666666666663</v>
+        <v>0.72916666666666663</v>
       </c>
       <c r="H100" t="str">
         <f t="shared" ref="H100:H109" si="76">VLOOKUP(A100,locations,2)</f>
@@ -4257,7 +4257,7 @@
         <v>45205</v>
       </c>
       <c r="E101" s="7">
-        <v>0.70833333333333337</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="F101" s="4">
         <f t="shared" si="15"/>
@@ -4265,7 +4265,7 @@
       </c>
       <c r="G101" s="5">
         <f t="shared" ref="G101:G103" si="78">E101+(1/24)</f>
-        <v>0.75</v>
+        <v>0.875</v>
       </c>
       <c r="H101" t="str">
         <f t="shared" si="76"/>
@@ -4281,7 +4281,7 @@
         <v>108</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>97</v>
+        <v>141</v>
       </c>
       <c r="C102" t="str">
         <f t="shared" si="1"/>
@@ -4325,15 +4325,15 @@
         <v>45206</v>
       </c>
       <c r="E103" s="7">
-        <v>0.72916666666666663</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F103" s="4">
         <f t="shared" si="15"/>
         <v>45206</v>
       </c>
       <c r="G103" s="5">
-        <f t="shared" si="78"/>
-        <v>0.77083333333333326</v>
+        <f>E103+(3*(1/96))</f>
+        <v>0.69791666666666663</v>
       </c>
       <c r="H103" t="str">
         <f t="shared" si="76"/>
@@ -4359,7 +4359,7 @@
         <v>45207</v>
       </c>
       <c r="E104" s="7">
-        <v>0.70833333333333337</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="F104" s="4">
         <f t="shared" si="15"/>
@@ -4367,7 +4367,7 @@
       </c>
       <c r="G104" s="5">
         <f t="shared" ref="G104" si="79">E104+(2*(1/24))</f>
-        <v>0.79166666666666674</v>
+        <v>0.91666666666666674</v>
       </c>
       <c r="H104" t="str">
         <f t="shared" si="76"/>
@@ -4451,7 +4451,7 @@
         <v>12</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>97</v>
+        <v>141</v>
       </c>
       <c r="C107" t="str">
         <f t="shared" si="1"/>
@@ -4461,15 +4461,15 @@
         <v>45220</v>
       </c>
       <c r="E107" s="7">
-        <v>0.54166666666666663</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="F107" s="4">
         <f t="shared" si="15"/>
         <v>45220</v>
       </c>
       <c r="G107" s="5">
-        <f t="shared" si="80"/>
-        <v>0.58333333333333326</v>
+        <f>E107+(3*(1/96))</f>
+        <v>0.55208333333333337</v>
       </c>
       <c r="H107" t="str">
         <f t="shared" si="76"/>
@@ -4791,7 +4791,7 @@
         <v>61</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>97</v>
+        <v>141</v>
       </c>
       <c r="C117" t="str">
         <f t="shared" si="1"/>
@@ -4801,15 +4801,15 @@
         <v>45234</v>
       </c>
       <c r="E117" s="5">
-        <v>0.47916666666666669</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="F117" s="4">
         <f t="shared" si="15"/>
         <v>45234</v>
       </c>
       <c r="G117" s="5">
-        <f t="shared" si="88"/>
-        <v>0.52083333333333337</v>
+        <f>E117+(3*(1/96))</f>
+        <v>0.48958333333333331</v>
       </c>
       <c r="H117" t="str">
         <f t="shared" si="86"/>

</xml_diff>

<commit_message>
Remove the Emilia Romagna Grand Prix
</commit_message>
<xml_diff>
--- a/f1/F1.xlsx
+++ b/f1/F1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin/projects/calendars/f1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03DB6C78-D5CE-A245-BFB5-AA900B61CD3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6590D0A-7A73-1D4D-B1BE-F2DEC5817C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3440" yWindow="780" windowWidth="28040" windowHeight="17440" xr2:uid="{65D0735D-D923-6F47-A559-767DB601EBAB}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="142">
   <si>
     <t>Country</t>
   </si>
@@ -947,11 +947,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A264AA3C-A8BA-6F48-8FC0-C3E78D3BD742}">
-  <dimension ref="A1:I129"/>
+  <dimension ref="A1:I124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G118" sqref="G118"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1233,7 +1231,7 @@
         <v>90</v>
       </c>
       <c r="C12" t="str">
-        <f t="shared" ref="C12:C129" si="1">VLOOKUP(A12,locations,4)</f>
+        <f t="shared" ref="C12:C124" si="1">VLOOKUP(A12,locations,4)</f>
         <v>Asia/Qatar</v>
       </c>
       <c r="D12" s="4">
@@ -1608,7 +1606,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="F23" s="4">
-        <f t="shared" ref="F23:F129" si="15">D23</f>
+        <f t="shared" ref="F23:F124" si="15">D23</f>
         <v>45003</v>
       </c>
       <c r="G23" s="5">
@@ -1616,7 +1614,7 @@
         <v>0.875</v>
       </c>
       <c r="H23" t="str">
-        <f t="shared" ref="H23:H128" si="16">VLOOKUP(A23,locations,2)</f>
+        <f t="shared" ref="H23:H123" si="16">VLOOKUP(A23,locations,2)</f>
         <v>Jeddah Corniche Circuit</v>
       </c>
       <c r="I23" t="str">
@@ -1790,7 +1788,7 @@
         <v>Melbourne Grand Prix Circuit</v>
       </c>
       <c r="I28" t="str">
-        <f t="shared" ref="I28:I128" si="20">VLOOKUP(A28,locations,3)</f>
+        <f t="shared" ref="I28:I123" si="20">VLOOKUP(A28,locations,3)</f>
         <v>Rolex Australian Grand Prix</v>
       </c>
     </row>
@@ -1820,11 +1818,11 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="H29" t="str">
-        <f t="shared" ref="H29:H42" si="22">VLOOKUP(A29,locations,2)</f>
+        <f t="shared" ref="H29:H33" si="22">VLOOKUP(A29,locations,2)</f>
         <v>Melbourne Grand Prix Circuit</v>
       </c>
       <c r="I29" t="str">
-        <f t="shared" ref="I29:I42" si="23">VLOOKUP(A29,locations,3)</f>
+        <f t="shared" ref="I29:I33" si="23">VLOOKUP(A29,locations,3)</f>
         <v>Rolex Australian Grand Prix</v>
       </c>
     </row>
@@ -1982,7 +1980,7 @@
         <v>0.625</v>
       </c>
       <c r="F34" s="4">
-        <f t="shared" ref="F34:F41" si="29">D34</f>
+        <f t="shared" ref="F34:F39" si="29">D34</f>
         <v>45046</v>
       </c>
       <c r="G34" s="5">
@@ -2160,170 +2158,170 @@
         <v>0.72916666666666674</v>
       </c>
       <c r="H39" t="str">
-        <f t="shared" ref="H39:H41" si="35">VLOOKUP(A39,locations,2)</f>
+        <f t="shared" ref="H39" si="35">VLOOKUP(A39,locations,2)</f>
         <v>Miami International Autodrome</v>
       </c>
       <c r="I39" t="str">
-        <f t="shared" ref="I39:I41" si="36">VLOOKUP(A39,locations,3)</f>
+        <f t="shared" ref="I39" si="36">VLOOKUP(A39,locations,3)</f>
         <v>crypto.com Miami Grand Prix</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Rome</v>
+        <v>Europe/Paris</v>
       </c>
       <c r="D40" s="4">
-        <v>45065</v>
+        <v>45072</v>
       </c>
       <c r="E40" s="5">
         <v>0.5625</v>
       </c>
       <c r="F40" s="4">
-        <f t="shared" si="29"/>
-        <v>45065</v>
+        <f t="shared" si="15"/>
+        <v>45072</v>
       </c>
       <c r="G40" s="5">
         <f>E40+(1/24)</f>
         <v>0.60416666666666663</v>
       </c>
       <c r="H40" t="str">
-        <f t="shared" si="35"/>
-        <v>Autodromo Enzo e Dino Ferrari</v>
+        <f t="shared" ref="H40:H42" si="37">VLOOKUP(A40,locations,2)</f>
+        <v>Circuit de Monaco</v>
       </c>
       <c r="I40" t="str">
-        <f t="shared" si="36"/>
-        <v>Gran Premio del Made In Italy e dell'Emilia Romagna</v>
+        <f t="shared" ref="I40:I42" si="38">VLOOKUP(A40,locations,3)</f>
+        <v>Grand Prix de Monaco</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>97</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Rome</v>
+        <v>Europe/Paris</v>
       </c>
       <c r="D41" s="4">
-        <v>45065</v>
+        <v>45072</v>
       </c>
       <c r="E41" s="5">
         <v>0.70833333333333337</v>
       </c>
       <c r="F41" s="4">
-        <f t="shared" si="29"/>
-        <v>45065</v>
+        <f t="shared" si="15"/>
+        <v>45072</v>
       </c>
       <c r="G41" s="5">
-        <f t="shared" ref="G41:G43" si="37">E41+(1/24)</f>
+        <f t="shared" ref="G41:G43" si="39">E41+(1/24)</f>
         <v>0.75</v>
       </c>
       <c r="H41" t="str">
-        <f t="shared" si="35"/>
-        <v>Autodromo Enzo e Dino Ferrari</v>
+        <f t="shared" si="37"/>
+        <v>Circuit de Monaco</v>
       </c>
       <c r="I41" t="str">
-        <f t="shared" si="36"/>
-        <v>Gran Premio del Made In Italy e dell'Emilia Romagna</v>
+        <f t="shared" si="38"/>
+        <v>Grand Prix de Monaco</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>98</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Rome</v>
+        <v>Europe/Paris</v>
       </c>
       <c r="D42" s="4">
-        <v>45066</v>
+        <v>45073</v>
       </c>
       <c r="E42" s="5">
         <v>0.52083333333333337</v>
       </c>
       <c r="F42" s="4">
         <f t="shared" si="15"/>
-        <v>45066</v>
+        <v>45073</v>
       </c>
       <c r="G42" s="5">
+        <f t="shared" si="39"/>
+        <v>0.5625</v>
+      </c>
+      <c r="H42" t="str">
         <f t="shared" si="37"/>
-        <v>0.5625</v>
-      </c>
-      <c r="H42" t="str">
-        <f t="shared" si="22"/>
-        <v>Autodromo Enzo e Dino Ferrari</v>
+        <v>Circuit de Monaco</v>
       </c>
       <c r="I42" t="str">
-        <f t="shared" si="23"/>
-        <v>Gran Premio del Made In Italy e dell'Emilia Romagna</v>
+        <f t="shared" si="38"/>
+        <v>Grand Prix de Monaco</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C43" t="str">
-        <f t="shared" si="1"/>
-        <v>Europe/Rome</v>
+        <f>VLOOKUP(A43,locations,4)</f>
+        <v>Europe/Paris</v>
       </c>
       <c r="D43" s="4">
-        <v>45066</v>
+        <v>45073</v>
       </c>
       <c r="E43" s="5">
         <v>0.66666666666666663</v>
       </c>
       <c r="F43" s="4">
-        <f t="shared" si="15"/>
-        <v>45066</v>
+        <f>D43</f>
+        <v>45073</v>
       </c>
       <c r="G43" s="5">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>0.70833333333333326</v>
       </c>
       <c r="H43" t="str">
-        <f t="shared" ref="H43" si="38">VLOOKUP(A43,locations,2)</f>
-        <v>Autodromo Enzo e Dino Ferrari</v>
+        <f>VLOOKUP(A43,locations,2)</f>
+        <v>Circuit de Monaco</v>
       </c>
       <c r="I43" t="str">
-        <f t="shared" ref="I43" si="39">VLOOKUP(A43,locations,3)</f>
-        <v>Gran Premio del Made In Italy e dell'Emilia Romagna</v>
+        <f>VLOOKUP(A43,locations,3)</f>
+        <v>Grand Prix de Monaco</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C44" t="str">
-        <f t="shared" si="1"/>
-        <v>Europe/Rome</v>
+        <f>VLOOKUP(A44,locations,4)</f>
+        <v>Europe/Paris</v>
       </c>
       <c r="D44" s="4">
-        <v>45067</v>
+        <v>45074</v>
       </c>
       <c r="E44" s="5">
         <v>0.625</v>
       </c>
       <c r="F44" s="4">
-        <f t="shared" si="15"/>
-        <v>45067</v>
+        <f>D44</f>
+        <v>45074</v>
       </c>
       <c r="G44" s="5">
         <f t="shared" ref="G44" si="40">E44+(2*(1/24))</f>
@@ -2331,33 +2329,33 @@
       </c>
       <c r="H44" t="str">
         <f t="shared" ref="H44:H47" si="41">VLOOKUP(A44,locations,2)</f>
-        <v>Autodromo Enzo e Dino Ferrari</v>
+        <v>Circuit de Monaco</v>
       </c>
       <c r="I44" t="str">
         <f t="shared" ref="I44:I47" si="42">VLOOKUP(A44,locations,3)</f>
-        <v>Gran Premio del Made In Italy e dell'Emilia Romagna</v>
+        <v>Grand Prix de Monaco</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Paris</v>
+        <v>Europe/Madrid</v>
       </c>
       <c r="D45" s="4">
-        <v>45072</v>
+        <v>45079</v>
       </c>
       <c r="E45" s="5">
         <v>0.5625</v>
       </c>
       <c r="F45" s="4">
-        <f t="shared" si="15"/>
-        <v>45072</v>
+        <f>D45</f>
+        <v>45079</v>
       </c>
       <c r="G45" s="5">
         <f>E45+(1/24)</f>
@@ -2365,33 +2363,33 @@
       </c>
       <c r="H45" t="str">
         <f t="shared" si="41"/>
-        <v>Circuit de Monaco</v>
+        <v>Circuit de Barcelona-Catalunya</v>
       </c>
       <c r="I45" t="str">
         <f t="shared" si="42"/>
-        <v>Grand Prix de Monaco</v>
+        <v>Gran Premio de España</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>97</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Paris</v>
+        <v>Europe/Madrid</v>
       </c>
       <c r="D46" s="4">
-        <v>45072</v>
+        <v>45079</v>
       </c>
       <c r="E46" s="5">
         <v>0.70833333333333337</v>
       </c>
       <c r="F46" s="4">
-        <f t="shared" si="15"/>
-        <v>45072</v>
+        <f>D46</f>
+        <v>45079</v>
       </c>
       <c r="G46" s="5">
         <f t="shared" ref="G46:G48" si="43">E46+(1/24)</f>
@@ -2399,33 +2397,33 @@
       </c>
       <c r="H46" t="str">
         <f t="shared" si="41"/>
-        <v>Circuit de Monaco</v>
+        <v>Circuit de Barcelona-Catalunya</v>
       </c>
       <c r="I46" t="str">
         <f t="shared" si="42"/>
-        <v>Grand Prix de Monaco</v>
+        <v>Gran Premio de España</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>98</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Paris</v>
+        <v>Europe/Madrid</v>
       </c>
       <c r="D47" s="4">
-        <v>45073</v>
+        <v>45080</v>
       </c>
       <c r="E47" s="5">
         <v>0.52083333333333337</v>
       </c>
       <c r="F47" s="4">
-        <f t="shared" si="15"/>
-        <v>45073</v>
+        <f>D47</f>
+        <v>45080</v>
       </c>
       <c r="G47" s="5">
         <f t="shared" si="43"/>
@@ -2433,2277 +2431,2277 @@
       </c>
       <c r="H47" t="str">
         <f t="shared" si="41"/>
-        <v>Circuit de Monaco</v>
+        <v>Circuit de Barcelona-Catalunya</v>
       </c>
       <c r="I47" t="str">
         <f t="shared" si="42"/>
-        <v>Grand Prix de Monaco</v>
+        <v>Gran Premio de España</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C48" t="str">
-        <f>VLOOKUP(A48,locations,4)</f>
-        <v>Europe/Paris</v>
+        <f t="shared" si="1"/>
+        <v>Europe/Madrid</v>
       </c>
       <c r="D48" s="4">
-        <v>45073</v>
+        <v>45080</v>
       </c>
       <c r="E48" s="5">
         <v>0.66666666666666663</v>
       </c>
       <c r="F48" s="4">
-        <f>D48</f>
-        <v>45073</v>
+        <f t="shared" si="15"/>
+        <v>45080</v>
       </c>
       <c r="G48" s="5">
         <f t="shared" si="43"/>
         <v>0.70833333333333326</v>
       </c>
       <c r="H48" t="str">
-        <f>VLOOKUP(A48,locations,2)</f>
-        <v>Circuit de Monaco</v>
+        <f t="shared" si="16"/>
+        <v>Circuit de Barcelona-Catalunya</v>
       </c>
       <c r="I48" t="str">
-        <f>VLOOKUP(A48,locations,3)</f>
-        <v>Grand Prix de Monaco</v>
+        <f t="shared" si="20"/>
+        <v>Gran Premio de España</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C49" t="str">
-        <f>VLOOKUP(A49,locations,4)</f>
-        <v>Europe/Paris</v>
+        <f t="shared" si="1"/>
+        <v>Europe/Madrid</v>
       </c>
       <c r="D49" s="4">
-        <v>45074</v>
+        <v>45081</v>
       </c>
       <c r="E49" s="5">
         <v>0.625</v>
       </c>
       <c r="F49" s="4">
-        <f>D49</f>
-        <v>45074</v>
+        <f t="shared" si="15"/>
+        <v>45081</v>
       </c>
       <c r="G49" s="5">
         <f t="shared" ref="G49" si="44">E49+(2*(1/24))</f>
         <v>0.70833333333333337</v>
       </c>
       <c r="H49" t="str">
-        <f t="shared" ref="H49:H52" si="45">VLOOKUP(A49,locations,2)</f>
-        <v>Circuit de Monaco</v>
+        <f t="shared" ref="H49" si="45">VLOOKUP(A49,locations,2)</f>
+        <v>Circuit de Barcelona-Catalunya</v>
       </c>
       <c r="I49" t="str">
-        <f t="shared" ref="I49:I52" si="46">VLOOKUP(A49,locations,3)</f>
-        <v>Grand Prix de Monaco</v>
+        <f t="shared" ref="I49" si="46">VLOOKUP(A49,locations,3)</f>
+        <v>Gran Premio de España</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Madrid</v>
+        <v>America/Montreal</v>
       </c>
       <c r="D50" s="4">
-        <v>45079</v>
+        <v>45093</v>
       </c>
       <c r="E50" s="5">
         <v>0.5625</v>
       </c>
       <c r="F50" s="4">
-        <f>D50</f>
-        <v>45079</v>
+        <f t="shared" si="15"/>
+        <v>45093</v>
       </c>
       <c r="G50" s="5">
         <f>E50+(1/24)</f>
         <v>0.60416666666666663</v>
       </c>
       <c r="H50" t="str">
-        <f t="shared" si="45"/>
-        <v>Circuit de Barcelona-Catalunya</v>
+        <f t="shared" ref="H50:H59" si="47">VLOOKUP(A50,locations,2)</f>
+        <v>Circuit Gilles-Villeneuve</v>
       </c>
       <c r="I50" t="str">
-        <f t="shared" si="46"/>
-        <v>Gran Premio de España</v>
+        <f t="shared" ref="I50:I59" si="48">VLOOKUP(A50,locations,3)</f>
+        <v>Grand Prix du Canada</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>97</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Madrid</v>
+        <v>America/Montreal</v>
       </c>
       <c r="D51" s="4">
-        <v>45079</v>
+        <v>45093</v>
       </c>
       <c r="E51" s="5">
         <v>0.70833333333333337</v>
       </c>
       <c r="F51" s="4">
-        <f>D51</f>
-        <v>45079</v>
+        <f t="shared" si="15"/>
+        <v>45093</v>
       </c>
       <c r="G51" s="5">
-        <f t="shared" ref="G51:G53" si="47">E51+(1/24)</f>
+        <f t="shared" ref="G51:G53" si="49">E51+(1/24)</f>
         <v>0.75</v>
       </c>
       <c r="H51" t="str">
-        <f t="shared" si="45"/>
-        <v>Circuit de Barcelona-Catalunya</v>
+        <f t="shared" si="47"/>
+        <v>Circuit Gilles-Villeneuve</v>
       </c>
       <c r="I51" t="str">
-        <f t="shared" si="46"/>
-        <v>Gran Premio de España</v>
+        <f t="shared" si="48"/>
+        <v>Grand Prix du Canada</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>98</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Madrid</v>
+        <v>America/Montreal</v>
       </c>
       <c r="D52" s="4">
-        <v>45080</v>
+        <v>45094</v>
       </c>
       <c r="E52" s="5">
         <v>0.52083333333333337</v>
       </c>
       <c r="F52" s="4">
-        <f>D52</f>
-        <v>45080</v>
+        <f t="shared" si="15"/>
+        <v>45094</v>
       </c>
       <c r="G52" s="5">
+        <f t="shared" si="49"/>
+        <v>0.5625</v>
+      </c>
+      <c r="H52" t="str">
         <f t="shared" si="47"/>
-        <v>0.5625</v>
-      </c>
-      <c r="H52" t="str">
-        <f t="shared" si="45"/>
-        <v>Circuit de Barcelona-Catalunya</v>
+        <v>Circuit Gilles-Villeneuve</v>
       </c>
       <c r="I52" t="str">
-        <f t="shared" si="46"/>
-        <v>Gran Premio de España</v>
+        <f t="shared" si="48"/>
+        <v>Grand Prix du Canada</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Madrid</v>
+        <v>America/Montreal</v>
       </c>
       <c r="D53" s="4">
-        <v>45080</v>
+        <v>45094</v>
       </c>
       <c r="E53" s="5">
         <v>0.66666666666666663</v>
       </c>
       <c r="F53" s="4">
         <f t="shared" si="15"/>
-        <v>45080</v>
+        <v>45094</v>
       </c>
       <c r="G53" s="5">
+        <f t="shared" si="49"/>
+        <v>0.70833333333333326</v>
+      </c>
+      <c r="H53" t="str">
         <f t="shared" si="47"/>
-        <v>0.70833333333333326</v>
-      </c>
-      <c r="H53" t="str">
-        <f t="shared" si="16"/>
-        <v>Circuit de Barcelona-Catalunya</v>
+        <v>Circuit Gilles-Villeneuve</v>
       </c>
       <c r="I53" t="str">
-        <f t="shared" si="20"/>
-        <v>Gran Premio de España</v>
+        <f t="shared" si="48"/>
+        <v>Grand Prix du Canada</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Madrid</v>
+        <v>America/Montreal</v>
       </c>
       <c r="D54" s="4">
-        <v>45081</v>
+        <v>45095</v>
       </c>
       <c r="E54" s="5">
-        <v>0.625</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="F54" s="4">
         <f t="shared" si="15"/>
-        <v>45081</v>
+        <v>45095</v>
       </c>
       <c r="G54" s="5">
-        <f t="shared" ref="G54" si="48">E54+(2*(1/24))</f>
-        <v>0.70833333333333337</v>
+        <f t="shared" ref="G54" si="50">E54+(2*(1/24))</f>
+        <v>0.66666666666666674</v>
       </c>
       <c r="H54" t="str">
-        <f t="shared" ref="H54" si="49">VLOOKUP(A54,locations,2)</f>
-        <v>Circuit de Barcelona-Catalunya</v>
+        <f t="shared" si="47"/>
+        <v>Circuit Gilles-Villeneuve</v>
       </c>
       <c r="I54" t="str">
-        <f t="shared" ref="I54" si="50">VLOOKUP(A54,locations,3)</f>
-        <v>Gran Premio de España</v>
+        <f t="shared" si="48"/>
+        <v>Grand Prix du Canada</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="1"/>
-        <v>America/Montreal</v>
+        <v>Europe/Vienna</v>
       </c>
       <c r="D55" s="4">
-        <v>45093</v>
+        <v>45107</v>
       </c>
       <c r="E55" s="5">
         <v>0.5625</v>
       </c>
       <c r="F55" s="4">
         <f t="shared" si="15"/>
-        <v>45093</v>
+        <v>45107</v>
       </c>
       <c r="G55" s="5">
         <f>E55+(1/24)</f>
         <v>0.60416666666666663</v>
       </c>
       <c r="H55" t="str">
-        <f t="shared" ref="H55:H64" si="51">VLOOKUP(A55,locations,2)</f>
-        <v>Circuit Gilles-Villeneuve</v>
+        <f t="shared" si="47"/>
+        <v>Red Bull Ring</v>
       </c>
       <c r="I55" t="str">
-        <f t="shared" ref="I55:I64" si="52">VLOOKUP(A55,locations,3)</f>
-        <v>Grand Prix du Canada</v>
+        <f t="shared" si="48"/>
+        <v>Grosser Preis von Österreich</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>97</v>
+        <v>11</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="1"/>
-        <v>America/Montreal</v>
+        <v>Europe/Vienna</v>
       </c>
       <c r="D56" s="4">
-        <v>45093</v>
+        <v>45107</v>
       </c>
       <c r="E56" s="5">
         <v>0.70833333333333337</v>
       </c>
       <c r="F56" s="4">
         <f t="shared" si="15"/>
-        <v>45093</v>
+        <v>45107</v>
       </c>
       <c r="G56" s="5">
-        <f t="shared" ref="G56:G58" si="53">E56+(1/24)</f>
+        <f t="shared" ref="G56:G58" si="51">E56+(1/24)</f>
         <v>0.75</v>
       </c>
       <c r="H56" t="str">
-        <f t="shared" si="51"/>
-        <v>Circuit Gilles-Villeneuve</v>
+        <f t="shared" si="47"/>
+        <v>Red Bull Ring</v>
       </c>
       <c r="I56" t="str">
-        <f t="shared" si="52"/>
-        <v>Grand Prix du Canada</v>
+        <f t="shared" si="48"/>
+        <v>Grosser Preis von Österreich</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>98</v>
+        <v>141</v>
       </c>
       <c r="C57" t="str">
-        <f t="shared" si="1"/>
-        <v>America/Montreal</v>
+        <f>VLOOKUP(A57,locations,4)</f>
+        <v>Europe/Vienna</v>
       </c>
       <c r="D57" s="4">
-        <v>45094</v>
+        <v>45108</v>
       </c>
       <c r="E57" s="5">
-        <v>0.52083333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="F57" s="4">
-        <f t="shared" si="15"/>
-        <v>45094</v>
+        <f t="shared" ref="F57:F62" si="52">D57</f>
+        <v>45108</v>
       </c>
       <c r="G57" s="5">
-        <f t="shared" si="53"/>
-        <v>0.5625</v>
+        <f>E57+(3*(1/96))</f>
+        <v>0.53125</v>
       </c>
       <c r="H57" t="str">
-        <f t="shared" si="51"/>
-        <v>Circuit Gilles-Villeneuve</v>
+        <f t="shared" si="47"/>
+        <v>Red Bull Ring</v>
       </c>
       <c r="I57" t="str">
-        <f t="shared" si="52"/>
-        <v>Grand Prix du Canada</v>
+        <f t="shared" si="48"/>
+        <v>Grosser Preis von Österreich</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="C58" t="str">
-        <f t="shared" si="1"/>
-        <v>America/Montreal</v>
+        <f>VLOOKUP(A58,locations,4)</f>
+        <v>Europe/Vienna</v>
       </c>
       <c r="D58" s="4">
-        <v>45094</v>
+        <v>45108</v>
       </c>
       <c r="E58" s="5">
-        <v>0.66666666666666663</v>
+        <v>0.6875</v>
       </c>
       <c r="F58" s="4">
-        <f t="shared" si="15"/>
-        <v>45094</v>
+        <f t="shared" si="52"/>
+        <v>45108</v>
       </c>
       <c r="G58" s="5">
-        <f t="shared" si="53"/>
-        <v>0.70833333333333326</v>
+        <f t="shared" si="51"/>
+        <v>0.72916666666666663</v>
       </c>
       <c r="H58" t="str">
-        <f t="shared" si="51"/>
-        <v>Circuit Gilles-Villeneuve</v>
+        <f t="shared" si="47"/>
+        <v>Red Bull Ring</v>
       </c>
       <c r="I58" t="str">
-        <f t="shared" si="52"/>
-        <v>Grand Prix du Canada</v>
+        <f t="shared" si="48"/>
+        <v>Grosser Preis von Österreich</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C59" t="str">
-        <f t="shared" si="1"/>
-        <v>America/Montreal</v>
+        <f>VLOOKUP(A59,locations,4)</f>
+        <v>Europe/Vienna</v>
       </c>
       <c r="D59" s="4">
-        <v>45095</v>
+        <v>45109</v>
       </c>
       <c r="E59" s="5">
-        <v>0.58333333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="F59" s="4">
-        <f t="shared" si="15"/>
-        <v>45095</v>
+        <f t="shared" si="52"/>
+        <v>45109</v>
       </c>
       <c r="G59" s="5">
-        <f t="shared" ref="G59" si="54">E59+(2*(1/24))</f>
-        <v>0.66666666666666674</v>
+        <f t="shared" ref="G59" si="53">E59+(2*(1/24))</f>
+        <v>0.70833333333333337</v>
       </c>
       <c r="H59" t="str">
-        <f t="shared" si="51"/>
-        <v>Circuit Gilles-Villeneuve</v>
+        <f t="shared" si="47"/>
+        <v>Red Bull Ring</v>
       </c>
       <c r="I59" t="str">
-        <f t="shared" si="52"/>
-        <v>Grand Prix du Canada</v>
+        <f t="shared" si="48"/>
+        <v>Grosser Preis von Österreich</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Vienna</v>
+        <v>Europe/London</v>
       </c>
       <c r="D60" s="4">
-        <v>45107</v>
+        <v>45114</v>
       </c>
       <c r="E60" s="5">
-        <v>0.5625</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="F60" s="4">
-        <f t="shared" si="15"/>
-        <v>45107</v>
+        <f t="shared" si="52"/>
+        <v>45114</v>
       </c>
       <c r="G60" s="5">
         <f>E60+(1/24)</f>
-        <v>0.60416666666666663</v>
+        <v>0.5625</v>
       </c>
       <c r="H60" t="str">
-        <f t="shared" si="51"/>
-        <v>Red Bull Ring</v>
+        <f t="shared" ref="H60:H79" si="54">VLOOKUP(A60,locations,2)</f>
+        <v>Silverstone</v>
       </c>
       <c r="I60" t="str">
-        <f t="shared" si="52"/>
-        <v>Grosser Preis von Österreich</v>
+        <f t="shared" ref="I60:I79" si="55">VLOOKUP(A60,locations,3)</f>
+        <v>Aramco British Grand Prix</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>11</v>
+        <v>97</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Vienna</v>
+        <v>Europe/London</v>
       </c>
       <c r="D61" s="4">
-        <v>45107</v>
+        <v>45114</v>
       </c>
       <c r="E61" s="5">
-        <v>0.70833333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F61" s="4">
-        <f t="shared" si="15"/>
-        <v>45107</v>
+        <f t="shared" si="52"/>
+        <v>45114</v>
       </c>
       <c r="G61" s="5">
-        <f t="shared" ref="G61:G63" si="55">E61+(1/24)</f>
-        <v>0.75</v>
+        <f t="shared" ref="G61:G63" si="56">E61+(1/24)</f>
+        <v>0.70833333333333326</v>
       </c>
       <c r="H61" t="str">
-        <f t="shared" si="51"/>
-        <v>Red Bull Ring</v>
+        <f t="shared" si="54"/>
+        <v>Silverstone</v>
       </c>
       <c r="I61" t="str">
-        <f t="shared" si="52"/>
-        <v>Grosser Preis von Österreich</v>
+        <f t="shared" si="55"/>
+        <v>Aramco British Grand Prix</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>141</v>
+        <v>98</v>
       </c>
       <c r="C62" t="str">
-        <f>VLOOKUP(A62,locations,4)</f>
-        <v>Europe/Vienna</v>
+        <f t="shared" si="1"/>
+        <v>Europe/London</v>
       </c>
       <c r="D62" s="4">
-        <v>45108</v>
+        <v>45115</v>
       </c>
       <c r="E62" s="5">
-        <v>0.5</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="F62" s="4">
-        <f t="shared" ref="F62:F67" si="56">D62</f>
-        <v>45108</v>
+        <f t="shared" si="52"/>
+        <v>45115</v>
       </c>
       <c r="G62" s="5">
-        <f>E62+(3*(1/96))</f>
-        <v>0.53125</v>
+        <f t="shared" si="56"/>
+        <v>0.52083333333333337</v>
       </c>
       <c r="H62" t="str">
-        <f t="shared" si="51"/>
-        <v>Red Bull Ring</v>
+        <f t="shared" si="54"/>
+        <v>Silverstone</v>
       </c>
       <c r="I62" t="str">
-        <f t="shared" si="52"/>
-        <v>Grosser Preis von Österreich</v>
+        <f t="shared" si="55"/>
+        <v>Aramco British Grand Prix</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>88</v>
+        <v>11</v>
       </c>
       <c r="C63" t="str">
-        <f>VLOOKUP(A63,locations,4)</f>
-        <v>Europe/Vienna</v>
+        <f t="shared" si="1"/>
+        <v>Europe/London</v>
       </c>
       <c r="D63" s="4">
-        <v>45108</v>
+        <v>45115</v>
       </c>
       <c r="E63" s="5">
-        <v>0.6875</v>
+        <v>0.625</v>
       </c>
       <c r="F63" s="4">
+        <f t="shared" si="15"/>
+        <v>45115</v>
+      </c>
+      <c r="G63" s="5">
         <f t="shared" si="56"/>
-        <v>45108</v>
-      </c>
-      <c r="G63" s="5">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H63" t="str">
+        <f t="shared" si="54"/>
+        <v>Silverstone</v>
+      </c>
+      <c r="I63" t="str">
         <f t="shared" si="55"/>
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="H63" t="str">
-        <f t="shared" si="51"/>
-        <v>Red Bull Ring</v>
-      </c>
-      <c r="I63" t="str">
-        <f t="shared" si="52"/>
-        <v>Grosser Preis von Österreich</v>
+        <v>Aramco British Grand Prix</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C64" t="str">
-        <f>VLOOKUP(A64,locations,4)</f>
-        <v>Europe/Vienna</v>
+        <f t="shared" si="1"/>
+        <v>Europe/London</v>
       </c>
       <c r="D64" s="4">
-        <v>45109</v>
+        <v>45116</v>
       </c>
       <c r="E64" s="5">
         <v>0.625</v>
       </c>
       <c r="F64" s="4">
-        <f t="shared" si="56"/>
-        <v>45109</v>
+        <f t="shared" si="15"/>
+        <v>45116</v>
       </c>
       <c r="G64" s="5">
         <f t="shared" ref="G64" si="57">E64+(2*(1/24))</f>
         <v>0.70833333333333337</v>
       </c>
       <c r="H64" t="str">
-        <f t="shared" si="51"/>
-        <v>Red Bull Ring</v>
+        <f t="shared" si="54"/>
+        <v>Silverstone</v>
       </c>
       <c r="I64" t="str">
-        <f t="shared" si="52"/>
-        <v>Grosser Preis von Österreich</v>
+        <f t="shared" si="55"/>
+        <v>Aramco British Grand Prix</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/London</v>
+        <v>Europe/Budapest</v>
       </c>
       <c r="D65" s="4">
-        <v>45114</v>
+        <v>45128</v>
       </c>
       <c r="E65" s="5">
-        <v>0.52083333333333337</v>
+        <v>0.5625</v>
       </c>
       <c r="F65" s="4">
-        <f t="shared" si="56"/>
-        <v>45114</v>
+        <f t="shared" si="15"/>
+        <v>45128</v>
       </c>
       <c r="G65" s="5">
         <f>E65+(1/24)</f>
-        <v>0.5625</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="H65" t="str">
-        <f t="shared" ref="H65:H84" si="58">VLOOKUP(A65,locations,2)</f>
-        <v>Silverstone</v>
+        <f t="shared" si="54"/>
+        <v>Hungaroring</v>
       </c>
       <c r="I65" t="str">
-        <f t="shared" ref="I65:I84" si="59">VLOOKUP(A65,locations,3)</f>
-        <v>Aramco British Grand Prix</v>
+        <f t="shared" si="55"/>
+        <v>Magyar Nagydíj</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>97</v>
       </c>
       <c r="C66" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/London</v>
+        <v>Europe/Budapest</v>
       </c>
       <c r="D66" s="4">
-        <v>45114</v>
+        <v>45128</v>
       </c>
       <c r="E66" s="5">
-        <v>0.66666666666666663</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="F66" s="4">
-        <f t="shared" si="56"/>
-        <v>45114</v>
+        <f t="shared" si="15"/>
+        <v>45128</v>
       </c>
       <c r="G66" s="5">
-        <f t="shared" ref="G66:G68" si="60">E66+(1/24)</f>
-        <v>0.70833333333333326</v>
+        <f t="shared" ref="G66:G68" si="58">E66+(1/24)</f>
+        <v>0.75</v>
       </c>
       <c r="H66" t="str">
-        <f t="shared" si="58"/>
-        <v>Silverstone</v>
+        <f t="shared" si="54"/>
+        <v>Hungaroring</v>
       </c>
       <c r="I66" t="str">
-        <f t="shared" si="59"/>
-        <v>Aramco British Grand Prix</v>
+        <f t="shared" si="55"/>
+        <v>Magyar Nagydíj</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>98</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/London</v>
+        <v>Europe/Budapest</v>
       </c>
       <c r="D67" s="4">
-        <v>45115</v>
+        <v>45129</v>
       </c>
       <c r="E67" s="5">
-        <v>0.47916666666666669</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="F67" s="4">
-        <f t="shared" si="56"/>
-        <v>45115</v>
+        <f t="shared" si="15"/>
+        <v>45129</v>
       </c>
       <c r="G67" s="5">
-        <f t="shared" si="60"/>
-        <v>0.52083333333333337</v>
+        <f t="shared" si="58"/>
+        <v>0.5625</v>
       </c>
       <c r="H67" t="str">
-        <f t="shared" si="58"/>
-        <v>Silverstone</v>
+        <f t="shared" si="54"/>
+        <v>Hungaroring</v>
       </c>
       <c r="I67" t="str">
-        <f t="shared" si="59"/>
-        <v>Aramco British Grand Prix</v>
+        <f t="shared" si="55"/>
+        <v>Magyar Nagydíj</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/London</v>
+        <v>Europe/Budapest</v>
       </c>
       <c r="D68" s="4">
-        <v>45115</v>
+        <v>45129</v>
       </c>
       <c r="E68" s="5">
-        <v>0.625</v>
+        <v>0.6875</v>
       </c>
       <c r="F68" s="4">
         <f t="shared" si="15"/>
-        <v>45115</v>
+        <v>45129</v>
       </c>
       <c r="G68" s="5">
-        <f t="shared" si="60"/>
-        <v>0.66666666666666663</v>
+        <f t="shared" si="58"/>
+        <v>0.72916666666666663</v>
       </c>
       <c r="H68" t="str">
-        <f t="shared" si="58"/>
-        <v>Silverstone</v>
+        <f t="shared" si="54"/>
+        <v>Hungaroring</v>
       </c>
       <c r="I68" t="str">
-        <f t="shared" si="59"/>
-        <v>Aramco British Grand Prix</v>
+        <f t="shared" si="55"/>
+        <v>Magyar Nagydíj</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/London</v>
+        <v>Europe/Budapest</v>
       </c>
       <c r="D69" s="4">
-        <v>45116</v>
+        <v>45130</v>
       </c>
       <c r="E69" s="5">
         <v>0.625</v>
       </c>
       <c r="F69" s="4">
         <f t="shared" si="15"/>
-        <v>45116</v>
+        <v>45130</v>
       </c>
       <c r="G69" s="5">
-        <f t="shared" ref="G69" si="61">E69+(2*(1/24))</f>
+        <f t="shared" ref="G69" si="59">E69+(2*(1/24))</f>
         <v>0.70833333333333337</v>
       </c>
       <c r="H69" t="str">
-        <f t="shared" si="58"/>
-        <v>Silverstone</v>
+        <f t="shared" si="54"/>
+        <v>Hungaroring</v>
       </c>
       <c r="I69" t="str">
-        <f t="shared" si="59"/>
-        <v>Aramco British Grand Prix</v>
+        <f t="shared" si="55"/>
+        <v>Magyar Nagydíj</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Budapest</v>
+        <v>Europe/Brussels</v>
       </c>
       <c r="D70" s="4">
-        <v>45128</v>
+        <v>45135</v>
       </c>
       <c r="E70" s="5">
         <v>0.5625</v>
       </c>
       <c r="F70" s="4">
         <f t="shared" si="15"/>
-        <v>45128</v>
+        <v>45135</v>
       </c>
       <c r="G70" s="5">
         <f>E70+(1/24)</f>
         <v>0.60416666666666663</v>
       </c>
       <c r="H70" t="str">
-        <f t="shared" si="58"/>
-        <v>Hungaroring</v>
+        <f t="shared" si="54"/>
+        <v>Circuit de Spa-Francorchamps</v>
       </c>
       <c r="I70" t="str">
-        <f t="shared" si="59"/>
-        <v>Magyar Nagydíj</v>
+        <f t="shared" si="55"/>
+        <v>Belgian Grand Prix</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>97</v>
+        <v>11</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Budapest</v>
+        <v>Europe/Brussels</v>
       </c>
       <c r="D71" s="4">
-        <v>45128</v>
+        <v>45135</v>
       </c>
       <c r="E71" s="5">
         <v>0.70833333333333337</v>
       </c>
       <c r="F71" s="4">
         <f t="shared" si="15"/>
-        <v>45128</v>
+        <v>45135</v>
       </c>
       <c r="G71" s="5">
-        <f t="shared" ref="G71:G73" si="62">E71+(1/24)</f>
+        <f t="shared" ref="G71:G73" si="60">E71+(1/24)</f>
         <v>0.75</v>
       </c>
       <c r="H71" t="str">
-        <f t="shared" si="58"/>
-        <v>Hungaroring</v>
+        <f t="shared" si="54"/>
+        <v>Circuit de Spa-Francorchamps</v>
       </c>
       <c r="I71" t="str">
-        <f t="shared" si="59"/>
-        <v>Magyar Nagydíj</v>
+        <f t="shared" si="55"/>
+        <v>Belgian Grand Prix</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>98</v>
+        <v>141</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Budapest</v>
+        <v>Europe/Brussels</v>
       </c>
       <c r="D72" s="4">
-        <v>45129</v>
+        <v>45136</v>
       </c>
       <c r="E72" s="5">
-        <v>0.52083333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="F72" s="4">
         <f t="shared" si="15"/>
-        <v>45129</v>
+        <v>45136</v>
       </c>
       <c r="G72" s="5">
-        <f t="shared" si="62"/>
-        <v>0.5625</v>
+        <f>E72+(3*(1/96))</f>
+        <v>0.53125</v>
       </c>
       <c r="H72" t="str">
-        <f t="shared" si="58"/>
-        <v>Hungaroring</v>
+        <f t="shared" si="54"/>
+        <v>Circuit de Spa-Francorchamps</v>
       </c>
       <c r="I72" t="str">
-        <f t="shared" si="59"/>
-        <v>Magyar Nagydíj</v>
+        <f t="shared" si="55"/>
+        <v>Belgian Grand Prix</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Budapest</v>
+        <v>Europe/Brussels</v>
       </c>
       <c r="D73" s="4">
-        <v>45129</v>
+        <v>45136</v>
       </c>
       <c r="E73" s="5">
         <v>0.6875</v>
       </c>
       <c r="F73" s="4">
         <f t="shared" si="15"/>
-        <v>45129</v>
+        <v>45136</v>
       </c>
       <c r="G73" s="5">
-        <f t="shared" si="62"/>
+        <f t="shared" si="60"/>
         <v>0.72916666666666663</v>
       </c>
       <c r="H73" t="str">
-        <f t="shared" si="58"/>
-        <v>Hungaroring</v>
+        <f t="shared" si="54"/>
+        <v>Circuit de Spa-Francorchamps</v>
       </c>
       <c r="I73" t="str">
-        <f t="shared" si="59"/>
-        <v>Magyar Nagydíj</v>
+        <f t="shared" si="55"/>
+        <v>Belgian Grand Prix</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Budapest</v>
+        <v>Europe/Brussels</v>
       </c>
       <c r="D74" s="4">
-        <v>45130</v>
+        <v>45137</v>
       </c>
       <c r="E74" s="5">
         <v>0.625</v>
       </c>
       <c r="F74" s="4">
         <f t="shared" si="15"/>
-        <v>45130</v>
+        <v>45137</v>
       </c>
       <c r="G74" s="5">
-        <f t="shared" ref="G74" si="63">E74+(2*(1/24))</f>
+        <f t="shared" ref="G74" si="61">E74+(2*(1/24))</f>
         <v>0.70833333333333337</v>
       </c>
       <c r="H74" t="str">
-        <f t="shared" si="58"/>
-        <v>Hungaroring</v>
+        <f t="shared" si="54"/>
+        <v>Circuit de Spa-Francorchamps</v>
       </c>
       <c r="I74" t="str">
-        <f t="shared" si="59"/>
-        <v>Magyar Nagydíj</v>
+        <f t="shared" si="55"/>
+        <v>Belgian Grand Prix</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Brussels</v>
+        <v>Europe/Amsterdam</v>
       </c>
       <c r="D75" s="4">
-        <v>45135</v>
+        <v>45163</v>
       </c>
       <c r="E75" s="5">
-        <v>0.5625</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="F75" s="4">
         <f t="shared" si="15"/>
-        <v>45135</v>
+        <v>45163</v>
       </c>
       <c r="G75" s="5">
         <f>E75+(1/24)</f>
-        <v>0.60416666666666663</v>
+        <v>0.5625</v>
       </c>
       <c r="H75" t="str">
-        <f t="shared" si="58"/>
-        <v>Circuit de Spa-Francorchamps</v>
+        <f t="shared" si="54"/>
+        <v>Circuit Zandvoort</v>
       </c>
       <c r="I75" t="str">
-        <f t="shared" si="59"/>
-        <v>Belgian Grand Prix</v>
+        <f t="shared" si="55"/>
+        <v>Heineken Dutch Grand Prix</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>11</v>
+        <v>97</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Brussels</v>
+        <v>Europe/Amsterdam</v>
       </c>
       <c r="D76" s="4">
-        <v>45135</v>
+        <v>45163</v>
       </c>
       <c r="E76" s="5">
-        <v>0.70833333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F76" s="4">
         <f t="shared" si="15"/>
-        <v>45135</v>
+        <v>45163</v>
       </c>
       <c r="G76" s="5">
-        <f t="shared" ref="G76:G78" si="64">E76+(1/24)</f>
-        <v>0.75</v>
+        <f t="shared" ref="G76:G78" si="62">E76+(1/24)</f>
+        <v>0.70833333333333326</v>
       </c>
       <c r="H76" t="str">
-        <f t="shared" si="58"/>
-        <v>Circuit de Spa-Francorchamps</v>
+        <f t="shared" si="54"/>
+        <v>Circuit Zandvoort</v>
       </c>
       <c r="I76" t="str">
-        <f t="shared" si="59"/>
-        <v>Belgian Grand Prix</v>
+        <f t="shared" si="55"/>
+        <v>Heineken Dutch Grand Prix</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>141</v>
+        <v>98</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Brussels</v>
+        <v>Europe/Amsterdam</v>
       </c>
       <c r="D77" s="4">
-        <v>45136</v>
+        <v>45164</v>
       </c>
       <c r="E77" s="5">
-        <v>0.5</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="F77" s="4">
         <f t="shared" si="15"/>
-        <v>45136</v>
+        <v>45164</v>
       </c>
       <c r="G77" s="5">
-        <f>E77+(3*(1/96))</f>
-        <v>0.53125</v>
+        <f t="shared" si="62"/>
+        <v>0.52083333333333337</v>
       </c>
       <c r="H77" t="str">
-        <f t="shared" si="58"/>
-        <v>Circuit de Spa-Francorchamps</v>
+        <f t="shared" si="54"/>
+        <v>Circuit Zandvoort</v>
       </c>
       <c r="I77" t="str">
-        <f t="shared" si="59"/>
-        <v>Belgian Grand Prix</v>
+        <f t="shared" si="55"/>
+        <v>Heineken Dutch Grand Prix</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>88</v>
+        <v>11</v>
       </c>
       <c r="C78" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Brussels</v>
+        <v>Europe/Amsterdam</v>
       </c>
       <c r="D78" s="4">
-        <v>45136</v>
+        <v>45164</v>
       </c>
       <c r="E78" s="5">
-        <v>0.6875</v>
+        <v>0.625</v>
       </c>
       <c r="F78" s="4">
         <f t="shared" si="15"/>
-        <v>45136</v>
+        <v>45164</v>
       </c>
       <c r="G78" s="5">
-        <f t="shared" si="64"/>
-        <v>0.72916666666666663</v>
+        <f t="shared" si="62"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="H78" t="str">
-        <f t="shared" si="58"/>
-        <v>Circuit de Spa-Francorchamps</v>
+        <f t="shared" si="54"/>
+        <v>Circuit Zandvoort</v>
       </c>
       <c r="I78" t="str">
-        <f t="shared" si="59"/>
-        <v>Belgian Grand Prix</v>
+        <f t="shared" si="55"/>
+        <v>Heineken Dutch Grand Prix</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Brussels</v>
+        <v>Europe/Amsterdam</v>
       </c>
       <c r="D79" s="4">
-        <v>45137</v>
+        <v>45165</v>
       </c>
       <c r="E79" s="5">
         <v>0.625</v>
       </c>
       <c r="F79" s="4">
         <f t="shared" si="15"/>
-        <v>45137</v>
+        <v>45165</v>
       </c>
       <c r="G79" s="5">
-        <f t="shared" ref="G79" si="65">E79+(2*(1/24))</f>
+        <f t="shared" ref="G79" si="63">E79+(2*(1/24))</f>
         <v>0.70833333333333337</v>
       </c>
       <c r="H79" t="str">
-        <f t="shared" si="58"/>
-        <v>Circuit de Spa-Francorchamps</v>
+        <f t="shared" si="54"/>
+        <v>Circuit Zandvoort</v>
       </c>
       <c r="I79" t="str">
-        <f t="shared" si="59"/>
-        <v>Belgian Grand Prix</v>
+        <f t="shared" si="55"/>
+        <v>Heineken Dutch Grand Prix</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C80" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Amsterdam</v>
+        <v>Europe/Rome</v>
       </c>
       <c r="D80" s="4">
-        <v>45163</v>
+        <v>45170</v>
       </c>
       <c r="E80" s="5">
-        <v>0.52083333333333337</v>
+        <v>0.5625</v>
       </c>
       <c r="F80" s="4">
         <f t="shared" si="15"/>
-        <v>45163</v>
+        <v>45170</v>
       </c>
       <c r="G80" s="5">
         <f>E80+(1/24)</f>
-        <v>0.5625</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="H80" t="str">
-        <f t="shared" si="58"/>
-        <v>Circuit Zandvoort</v>
+        <f t="shared" ref="H80:H94" si="64">VLOOKUP(A80,locations,2)</f>
+        <v>Autodromo Nazionale Monza</v>
       </c>
       <c r="I80" t="str">
-        <f t="shared" si="59"/>
-        <v>Heineken Dutch Grand Prix</v>
+        <f t="shared" ref="I80:I94" si="65">VLOOKUP(A80,locations,3)</f>
+        <v>Gran Premio d'Italia</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>97</v>
       </c>
       <c r="C81" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Amsterdam</v>
+        <v>Europe/Rome</v>
       </c>
       <c r="D81" s="4">
-        <v>45163</v>
+        <v>45170</v>
       </c>
       <c r="E81" s="5">
-        <v>0.66666666666666663</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="F81" s="4">
         <f t="shared" si="15"/>
-        <v>45163</v>
+        <v>45170</v>
       </c>
       <c r="G81" s="5">
         <f t="shared" ref="G81:G83" si="66">E81+(1/24)</f>
-        <v>0.70833333333333326</v>
+        <v>0.75</v>
       </c>
       <c r="H81" t="str">
-        <f t="shared" si="58"/>
-        <v>Circuit Zandvoort</v>
+        <f t="shared" si="64"/>
+        <v>Autodromo Nazionale Monza</v>
       </c>
       <c r="I81" t="str">
-        <f t="shared" si="59"/>
-        <v>Heineken Dutch Grand Prix</v>
+        <f t="shared" si="65"/>
+        <v>Gran Premio d'Italia</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>98</v>
       </c>
       <c r="C82" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Amsterdam</v>
+        <v>Europe/Rome</v>
       </c>
       <c r="D82" s="4">
-        <v>45164</v>
+        <v>45171</v>
       </c>
       <c r="E82" s="5">
-        <v>0.47916666666666669</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="F82" s="4">
         <f t="shared" si="15"/>
-        <v>45164</v>
+        <v>45171</v>
       </c>
       <c r="G82" s="5">
         <f t="shared" si="66"/>
-        <v>0.52083333333333337</v>
+        <v>0.5625</v>
       </c>
       <c r="H82" t="str">
-        <f t="shared" si="58"/>
-        <v>Circuit Zandvoort</v>
+        <f t="shared" si="64"/>
+        <v>Autodromo Nazionale Monza</v>
       </c>
       <c r="I82" t="str">
-        <f t="shared" si="59"/>
-        <v>Heineken Dutch Grand Prix</v>
+        <f t="shared" si="65"/>
+        <v>Gran Premio d'Italia</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C83" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Amsterdam</v>
+        <v>Europe/Rome</v>
       </c>
       <c r="D83" s="4">
-        <v>45164</v>
+        <v>45171</v>
       </c>
       <c r="E83" s="5">
-        <v>0.625</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F83" s="4">
         <f t="shared" si="15"/>
-        <v>45164</v>
+        <v>45171</v>
       </c>
       <c r="G83" s="5">
         <f t="shared" si="66"/>
-        <v>0.66666666666666663</v>
+        <v>0.70833333333333326</v>
       </c>
       <c r="H83" t="str">
-        <f t="shared" si="58"/>
-        <v>Circuit Zandvoort</v>
+        <f t="shared" si="64"/>
+        <v>Autodromo Nazionale Monza</v>
       </c>
       <c r="I83" t="str">
-        <f t="shared" si="59"/>
-        <v>Heineken Dutch Grand Prix</v>
+        <f t="shared" si="65"/>
+        <v>Gran Premio d'Italia</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C84" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Amsterdam</v>
+        <v>Europe/Rome</v>
       </c>
       <c r="D84" s="4">
-        <v>45165</v>
+        <v>45172</v>
       </c>
       <c r="E84" s="5">
         <v>0.625</v>
       </c>
       <c r="F84" s="4">
         <f t="shared" si="15"/>
-        <v>45165</v>
+        <v>45172</v>
       </c>
       <c r="G84" s="5">
         <f t="shared" ref="G84" si="67">E84+(2*(1/24))</f>
         <v>0.70833333333333337</v>
       </c>
       <c r="H84" t="str">
-        <f t="shared" si="58"/>
-        <v>Circuit Zandvoort</v>
+        <f t="shared" si="64"/>
+        <v>Autodromo Nazionale Monza</v>
       </c>
       <c r="I84" t="str">
-        <f t="shared" si="59"/>
-        <v>Heineken Dutch Grand Prix</v>
+        <f t="shared" si="65"/>
+        <v>Gran Premio d'Italia</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C85" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Rome</v>
+        <v>Asia/Singapore</v>
       </c>
       <c r="D85" s="4">
-        <v>45170</v>
+        <v>45184</v>
       </c>
       <c r="E85" s="5">
-        <v>0.5625</v>
+        <v>0.72916666666666663</v>
       </c>
       <c r="F85" s="4">
         <f t="shared" si="15"/>
-        <v>45170</v>
+        <v>45184</v>
       </c>
       <c r="G85" s="5">
         <f>E85+(1/24)</f>
-        <v>0.60416666666666663</v>
+        <v>0.77083333333333326</v>
       </c>
       <c r="H85" t="str">
-        <f t="shared" ref="H85:H99" si="68">VLOOKUP(A85,locations,2)</f>
-        <v>Autodromo Nazionale Monza</v>
+        <f t="shared" si="64"/>
+        <v>Marina Bay Street Circuit</v>
       </c>
       <c r="I85" t="str">
-        <f t="shared" ref="I85:I99" si="69">VLOOKUP(A85,locations,3)</f>
-        <v>Gran Premio d'Italia</v>
+        <f t="shared" si="65"/>
+        <v>Singapore Airlines Singapore Grand Prix</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>97</v>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Rome</v>
+        <v>Asia/Singapore</v>
       </c>
       <c r="D86" s="4">
-        <v>45170</v>
+        <v>45184</v>
       </c>
       <c r="E86" s="5">
-        <v>0.70833333333333337</v>
+        <v>0.875</v>
       </c>
       <c r="F86" s="4">
         <f t="shared" si="15"/>
-        <v>45170</v>
+        <v>45184</v>
       </c>
       <c r="G86" s="5">
-        <f t="shared" ref="G86:G88" si="70">E86+(1/24)</f>
-        <v>0.75</v>
+        <f t="shared" ref="G86:G88" si="68">E86+(1/24)</f>
+        <v>0.91666666666666663</v>
       </c>
       <c r="H86" t="str">
-        <f t="shared" si="68"/>
-        <v>Autodromo Nazionale Monza</v>
+        <f t="shared" si="64"/>
+        <v>Marina Bay Street Circuit</v>
       </c>
       <c r="I86" t="str">
-        <f t="shared" si="69"/>
-        <v>Gran Premio d'Italia</v>
+        <f t="shared" si="65"/>
+        <v>Singapore Airlines Singapore Grand Prix</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>98</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Rome</v>
+        <v>Asia/Singapore</v>
       </c>
       <c r="D87" s="4">
-        <v>45171</v>
+        <v>45185</v>
       </c>
       <c r="E87" s="5">
-        <v>0.52083333333333337</v>
+        <v>0.72916666666666663</v>
       </c>
       <c r="F87" s="4">
         <f t="shared" si="15"/>
-        <v>45171</v>
+        <v>45185</v>
       </c>
       <c r="G87" s="5">
-        <f t="shared" si="70"/>
-        <v>0.5625</v>
+        <f t="shared" si="68"/>
+        <v>0.77083333333333326</v>
       </c>
       <c r="H87" t="str">
-        <f t="shared" si="68"/>
-        <v>Autodromo Nazionale Monza</v>
+        <f t="shared" si="64"/>
+        <v>Marina Bay Street Circuit</v>
       </c>
       <c r="I87" t="str">
-        <f t="shared" si="69"/>
-        <v>Gran Premio d'Italia</v>
+        <f t="shared" si="65"/>
+        <v>Singapore Airlines Singapore Grand Prix</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C88" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Rome</v>
+        <v>Asia/Singapore</v>
       </c>
       <c r="D88" s="4">
-        <v>45171</v>
+        <v>45185</v>
       </c>
       <c r="E88" s="5">
-        <v>0.66666666666666663</v>
+        <v>0.875</v>
       </c>
       <c r="F88" s="4">
         <f t="shared" si="15"/>
-        <v>45171</v>
+        <v>45185</v>
       </c>
       <c r="G88" s="5">
-        <f t="shared" si="70"/>
-        <v>0.70833333333333326</v>
+        <f t="shared" si="68"/>
+        <v>0.91666666666666663</v>
       </c>
       <c r="H88" t="str">
-        <f t="shared" si="68"/>
-        <v>Autodromo Nazionale Monza</v>
+        <f t="shared" si="64"/>
+        <v>Marina Bay Street Circuit</v>
       </c>
       <c r="I88" t="str">
-        <f t="shared" si="69"/>
-        <v>Gran Premio d'Italia</v>
+        <f t="shared" si="65"/>
+        <v>Singapore Airlines Singapore Grand Prix</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C89" t="str">
         <f t="shared" si="1"/>
-        <v>Europe/Rome</v>
+        <v>Asia/Singapore</v>
       </c>
       <c r="D89" s="4">
-        <v>45172</v>
+        <v>45186</v>
       </c>
       <c r="E89" s="5">
-        <v>0.625</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="F89" s="4">
         <f t="shared" si="15"/>
-        <v>45172</v>
+        <v>45186</v>
       </c>
       <c r="G89" s="5">
-        <f t="shared" ref="G89" si="71">E89+(2*(1/24))</f>
-        <v>0.70833333333333337</v>
+        <f t="shared" ref="G89" si="69">E89+(2*(1/24))</f>
+        <v>0.91666666666666674</v>
       </c>
       <c r="H89" t="str">
-        <f t="shared" si="68"/>
-        <v>Autodromo Nazionale Monza</v>
+        <f t="shared" si="64"/>
+        <v>Marina Bay Street Circuit</v>
       </c>
       <c r="I89" t="str">
-        <f t="shared" si="69"/>
-        <v>Gran Premio d'Italia</v>
+        <f t="shared" si="65"/>
+        <v>Singapore Airlines Singapore Grand Prix</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="1"/>
-        <v>Asia/Singapore</v>
+        <v>Asia/Tokyo</v>
       </c>
       <c r="D90" s="4">
-        <v>45184</v>
+        <v>45191</v>
       </c>
       <c r="E90" s="5">
-        <v>0.72916666666666663</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="F90" s="4">
         <f t="shared" si="15"/>
-        <v>45184</v>
+        <v>45191</v>
       </c>
       <c r="G90" s="5">
         <f>E90+(1/24)</f>
-        <v>0.77083333333333326</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="H90" t="str">
-        <f t="shared" si="68"/>
-        <v>Marina Bay Street Circuit</v>
+        <f t="shared" si="64"/>
+        <v>Suzuka International Racing Course</v>
       </c>
       <c r="I90" t="str">
-        <f t="shared" si="69"/>
-        <v>Singapore Airlines Singapore Grand Prix</v>
+        <f t="shared" si="65"/>
+        <v>Lenovo Japanese Grand Prix</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>97</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="1"/>
-        <v>Asia/Singapore</v>
+        <v>Asia/Tokyo</v>
       </c>
       <c r="D91" s="4">
-        <v>45184</v>
+        <v>45191</v>
       </c>
       <c r="E91" s="5">
-        <v>0.875</v>
+        <v>0.625</v>
       </c>
       <c r="F91" s="4">
         <f t="shared" si="15"/>
-        <v>45184</v>
+        <v>45191</v>
       </c>
       <c r="G91" s="5">
-        <f t="shared" ref="G91:G93" si="72">E91+(1/24)</f>
-        <v>0.91666666666666663</v>
+        <f t="shared" ref="G91:G93" si="70">E91+(1/24)</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="H91" t="str">
-        <f t="shared" si="68"/>
-        <v>Marina Bay Street Circuit</v>
+        <f t="shared" si="64"/>
+        <v>Suzuka International Racing Course</v>
       </c>
       <c r="I91" t="str">
-        <f t="shared" si="69"/>
-        <v>Singapore Airlines Singapore Grand Prix</v>
+        <f t="shared" si="65"/>
+        <v>Lenovo Japanese Grand Prix</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>98</v>
       </c>
       <c r="C92" t="str">
         <f t="shared" si="1"/>
-        <v>Asia/Singapore</v>
+        <v>Asia/Tokyo</v>
       </c>
       <c r="D92" s="4">
-        <v>45185</v>
+        <v>45192</v>
       </c>
       <c r="E92" s="5">
-        <v>0.72916666666666663</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="F92" s="4">
         <f t="shared" si="15"/>
-        <v>45185</v>
+        <v>45192</v>
       </c>
       <c r="G92" s="5">
-        <f t="shared" si="72"/>
-        <v>0.77083333333333326</v>
+        <f t="shared" si="70"/>
+        <v>0.52083333333333337</v>
       </c>
       <c r="H92" t="str">
-        <f t="shared" si="68"/>
-        <v>Marina Bay Street Circuit</v>
+        <f t="shared" si="64"/>
+        <v>Suzuka International Racing Course</v>
       </c>
       <c r="I92" t="str">
-        <f t="shared" si="69"/>
-        <v>Singapore Airlines Singapore Grand Prix</v>
+        <f t="shared" si="65"/>
+        <v>Lenovo Japanese Grand Prix</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="1"/>
-        <v>Asia/Singapore</v>
+        <v>Asia/Tokyo</v>
       </c>
       <c r="D93" s="4">
-        <v>45185</v>
-      </c>
-      <c r="E93" s="5">
-        <v>0.875</v>
+        <v>45192</v>
+      </c>
+      <c r="E93" s="7">
+        <v>0.625</v>
       </c>
       <c r="F93" s="4">
         <f t="shared" si="15"/>
-        <v>45185</v>
+        <v>45192</v>
       </c>
       <c r="G93" s="5">
-        <f t="shared" si="72"/>
-        <v>0.91666666666666663</v>
+        <f t="shared" si="70"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="H93" t="str">
-        <f t="shared" si="68"/>
-        <v>Marina Bay Street Circuit</v>
+        <f t="shared" si="64"/>
+        <v>Suzuka International Racing Course</v>
       </c>
       <c r="I93" t="str">
-        <f t="shared" si="69"/>
-        <v>Singapore Airlines Singapore Grand Prix</v>
+        <f t="shared" si="65"/>
+        <v>Lenovo Japanese Grand Prix</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="1"/>
-        <v>Asia/Singapore</v>
+        <v>Asia/Tokyo</v>
       </c>
       <c r="D94" s="4">
-        <v>45186</v>
-      </c>
-      <c r="E94" s="5">
-        <v>0.83333333333333337</v>
+        <v>45193</v>
+      </c>
+      <c r="E94" s="7">
+        <v>0.58333333333333337</v>
       </c>
       <c r="F94" s="4">
         <f t="shared" si="15"/>
-        <v>45186</v>
+        <v>45193</v>
       </c>
       <c r="G94" s="5">
-        <f t="shared" ref="G94" si="73">E94+(2*(1/24))</f>
-        <v>0.91666666666666674</v>
+        <f t="shared" ref="G94" si="71">E94+(2*(1/24))</f>
+        <v>0.66666666666666674</v>
       </c>
       <c r="H94" t="str">
-        <f t="shared" si="68"/>
-        <v>Marina Bay Street Circuit</v>
+        <f t="shared" si="64"/>
+        <v>Suzuka International Racing Course</v>
       </c>
       <c r="I94" t="str">
-        <f t="shared" si="69"/>
-        <v>Singapore Airlines Singapore Grand Prix</v>
+        <f t="shared" si="65"/>
+        <v>Lenovo Japanese Grand Prix</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>19</v>
+        <v>108</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="1"/>
-        <v>Asia/Tokyo</v>
+        <v>Asia/Qatar</v>
       </c>
       <c r="D95" s="4">
-        <v>45191</v>
-      </c>
-      <c r="E95" s="5">
-        <v>0.47916666666666669</v>
+        <v>45205</v>
+      </c>
+      <c r="E95" s="7">
+        <v>0.6875</v>
       </c>
       <c r="F95" s="4">
         <f t="shared" si="15"/>
-        <v>45191</v>
+        <v>45205</v>
       </c>
       <c r="G95" s="5">
         <f>E95+(1/24)</f>
-        <v>0.52083333333333337</v>
+        <v>0.72916666666666663</v>
       </c>
       <c r="H95" t="str">
-        <f t="shared" si="68"/>
-        <v>Suzuka International Racing Course</v>
+        <f t="shared" ref="H95:H104" si="72">VLOOKUP(A95,locations,2)</f>
+        <v>Lusail International Circuit</v>
       </c>
       <c r="I95" t="str">
-        <f t="shared" si="69"/>
-        <v>Lenovo Japanese Grand Prix</v>
+        <f t="shared" ref="I95:I104" si="73">VLOOKUP(A95,locations,3)</f>
+        <v>Qatar Grand Prix</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>19</v>
+        <v>108</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>97</v>
+        <v>11</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="1"/>
-        <v>Asia/Tokyo</v>
+        <v>Asia/Qatar</v>
       </c>
       <c r="D96" s="4">
-        <v>45191</v>
-      </c>
-      <c r="E96" s="5">
-        <v>0.625</v>
+        <v>45205</v>
+      </c>
+      <c r="E96" s="7">
+        <v>0.83333333333333337</v>
       </c>
       <c r="F96" s="4">
         <f t="shared" si="15"/>
-        <v>45191</v>
+        <v>45205</v>
       </c>
       <c r="G96" s="5">
-        <f t="shared" ref="G96:G98" si="74">E96+(1/24)</f>
-        <v>0.66666666666666663</v>
+        <f t="shared" ref="G96:G97" si="74">E96+(1/24)</f>
+        <v>0.875</v>
       </c>
       <c r="H96" t="str">
-        <f t="shared" si="68"/>
-        <v>Suzuka International Racing Course</v>
+        <f t="shared" si="72"/>
+        <v>Lusail International Circuit</v>
       </c>
       <c r="I96" t="str">
-        <f t="shared" si="69"/>
-        <v>Lenovo Japanese Grand Prix</v>
+        <f t="shared" si="73"/>
+        <v>Qatar Grand Prix</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>19</v>
+        <v>108</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>98</v>
+        <v>141</v>
       </c>
       <c r="C97" t="str">
         <f t="shared" si="1"/>
-        <v>Asia/Tokyo</v>
+        <v>Asia/Qatar</v>
       </c>
       <c r="D97" s="4">
-        <v>45192</v>
-      </c>
-      <c r="E97" s="5">
-        <v>0.47916666666666669</v>
+        <v>45206</v>
+      </c>
+      <c r="E97" s="7">
+        <v>0.5625</v>
       </c>
       <c r="F97" s="4">
         <f t="shared" si="15"/>
-        <v>45192</v>
+        <v>45206</v>
       </c>
       <c r="G97" s="5">
         <f t="shared" si="74"/>
-        <v>0.52083333333333337</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="H97" t="str">
-        <f t="shared" si="68"/>
-        <v>Suzuka International Racing Course</v>
+        <f t="shared" si="72"/>
+        <v>Lusail International Circuit</v>
       </c>
       <c r="I97" t="str">
-        <f t="shared" si="69"/>
-        <v>Lenovo Japanese Grand Prix</v>
+        <f t="shared" si="73"/>
+        <v>Qatar Grand Prix</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>19</v>
+        <v>108</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="C98" t="str">
         <f t="shared" si="1"/>
-        <v>Asia/Tokyo</v>
+        <v>Asia/Qatar</v>
       </c>
       <c r="D98" s="4">
-        <v>45192</v>
+        <v>45206</v>
       </c>
       <c r="E98" s="7">
-        <v>0.625</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F98" s="4">
         <f t="shared" si="15"/>
-        <v>45192</v>
+        <v>45206</v>
       </c>
       <c r="G98" s="5">
-        <f t="shared" si="74"/>
-        <v>0.66666666666666663</v>
+        <f>E98+(3*(1/96))</f>
+        <v>0.69791666666666663</v>
       </c>
       <c r="H98" t="str">
-        <f t="shared" si="68"/>
-        <v>Suzuka International Racing Course</v>
+        <f t="shared" si="72"/>
+        <v>Lusail International Circuit</v>
       </c>
       <c r="I98" t="str">
-        <f t="shared" si="69"/>
-        <v>Lenovo Japanese Grand Prix</v>
+        <f t="shared" si="73"/>
+        <v>Qatar Grand Prix</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>19</v>
+        <v>108</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C99" t="str">
         <f t="shared" si="1"/>
-        <v>Asia/Tokyo</v>
+        <v>Asia/Qatar</v>
       </c>
       <c r="D99" s="4">
-        <v>45193</v>
+        <v>45207</v>
       </c>
       <c r="E99" s="7">
-        <v>0.58333333333333337</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="F99" s="4">
         <f t="shared" si="15"/>
-        <v>45193</v>
+        <v>45207</v>
       </c>
       <c r="G99" s="5">
         <f t="shared" ref="G99" si="75">E99+(2*(1/24))</f>
-        <v>0.66666666666666674</v>
+        <v>0.91666666666666674</v>
       </c>
       <c r="H99" t="str">
-        <f t="shared" si="68"/>
-        <v>Suzuka International Racing Course</v>
+        <f t="shared" si="72"/>
+        <v>Lusail International Circuit</v>
       </c>
       <c r="I99" t="str">
-        <f t="shared" si="69"/>
-        <v>Lenovo Japanese Grand Prix</v>
+        <f t="shared" si="73"/>
+        <v>Qatar Grand Prix</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C100" t="str">
         <f t="shared" si="1"/>
-        <v>Asia/Qatar</v>
+        <v>America/Chicago</v>
       </c>
       <c r="D100" s="4">
-        <v>45205</v>
+        <v>45219</v>
       </c>
       <c r="E100" s="7">
-        <v>0.6875</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="F100" s="4">
         <f t="shared" si="15"/>
-        <v>45205</v>
+        <v>45219</v>
       </c>
       <c r="G100" s="5">
         <f>E100+(1/24)</f>
-        <v>0.72916666666666663</v>
+        <v>0.5625</v>
       </c>
       <c r="H100" t="str">
-        <f t="shared" ref="H100:H109" si="76">VLOOKUP(A100,locations,2)</f>
-        <v>Lusail International Circuit</v>
+        <f t="shared" si="72"/>
+        <v>Circuit of The Americas</v>
       </c>
       <c r="I100" t="str">
-        <f t="shared" ref="I100:I109" si="77">VLOOKUP(A100,locations,3)</f>
-        <v>Qatar Grand Prix</v>
+        <f t="shared" si="73"/>
+        <v>Lenovo United States Grand Prix</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C101" t="str">
         <f t="shared" si="1"/>
-        <v>Asia/Qatar</v>
+        <v>America/Chicago</v>
       </c>
       <c r="D101" s="4">
-        <v>45205</v>
+        <v>45219</v>
       </c>
       <c r="E101" s="7">
-        <v>0.83333333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F101" s="4">
         <f t="shared" si="15"/>
-        <v>45205</v>
+        <v>45219</v>
       </c>
       <c r="G101" s="5">
-        <f t="shared" ref="G101:G103" si="78">E101+(1/24)</f>
-        <v>0.875</v>
+        <f t="shared" ref="G101:G103" si="76">E101+(1/24)</f>
+        <v>0.70833333333333326</v>
       </c>
       <c r="H101" t="str">
-        <f t="shared" si="76"/>
-        <v>Lusail International Circuit</v>
+        <f t="shared" si="72"/>
+        <v>Circuit of The Americas</v>
       </c>
       <c r="I101" t="str">
-        <f t="shared" si="77"/>
-        <v>Qatar Grand Prix</v>
+        <f t="shared" si="73"/>
+        <v>Lenovo United States Grand Prix</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>141</v>
       </c>
       <c r="C102" t="str">
         <f t="shared" si="1"/>
-        <v>Asia/Qatar</v>
+        <v>America/Chicago</v>
       </c>
       <c r="D102" s="4">
-        <v>45206</v>
+        <v>45220</v>
       </c>
       <c r="E102" s="7">
-        <v>0.5625</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="F102" s="4">
         <f t="shared" si="15"/>
-        <v>45206</v>
+        <v>45220</v>
       </c>
       <c r="G102" s="5">
-        <f t="shared" si="78"/>
-        <v>0.60416666666666663</v>
+        <f>E102+(3*(1/96))</f>
+        <v>0.55208333333333337</v>
       </c>
       <c r="H102" t="str">
-        <f t="shared" si="76"/>
-        <v>Lusail International Circuit</v>
+        <f t="shared" si="72"/>
+        <v>Circuit of The Americas</v>
       </c>
       <c r="I102" t="str">
-        <f t="shared" si="77"/>
-        <v>Qatar Grand Prix</v>
+        <f t="shared" si="73"/>
+        <v>Lenovo United States Grand Prix</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>88</v>
       </c>
       <c r="C103" t="str">
         <f t="shared" si="1"/>
-        <v>Asia/Qatar</v>
+        <v>America/Chicago</v>
       </c>
       <c r="D103" s="4">
-        <v>45206</v>
-      </c>
-      <c r="E103" s="7">
-        <v>0.66666666666666663</v>
+        <v>45220</v>
+      </c>
+      <c r="E103" s="5">
+        <v>0.70833333333333337</v>
       </c>
       <c r="F103" s="4">
         <f t="shared" si="15"/>
-        <v>45206</v>
+        <v>45220</v>
       </c>
       <c r="G103" s="5">
-        <f>E103+(3*(1/96))</f>
-        <v>0.69791666666666663</v>
+        <f t="shared" si="76"/>
+        <v>0.75</v>
       </c>
       <c r="H103" t="str">
-        <f t="shared" si="76"/>
-        <v>Lusail International Circuit</v>
+        <f t="shared" si="72"/>
+        <v>Circuit of The Americas</v>
       </c>
       <c r="I103" t="str">
-        <f t="shared" si="77"/>
-        <v>Qatar Grand Prix</v>
+        <f t="shared" si="73"/>
+        <v>Lenovo United States Grand Prix</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C104" t="str">
         <f t="shared" si="1"/>
-        <v>Asia/Qatar</v>
+        <v>America/Chicago</v>
       </c>
       <c r="D104" s="4">
-        <v>45207</v>
-      </c>
-      <c r="E104" s="7">
-        <v>0.83333333333333337</v>
+        <v>45221</v>
+      </c>
+      <c r="E104" s="5">
+        <v>0.58333333333333337</v>
       </c>
       <c r="F104" s="4">
         <f t="shared" si="15"/>
-        <v>45207</v>
+        <v>45221</v>
       </c>
       <c r="G104" s="5">
-        <f t="shared" ref="G104" si="79">E104+(2*(1/24))</f>
-        <v>0.91666666666666674</v>
+        <f t="shared" ref="G104" si="77">E104+(2*(1/24))</f>
+        <v>0.66666666666666674</v>
       </c>
       <c r="H104" t="str">
-        <f t="shared" si="76"/>
-        <v>Lusail International Circuit</v>
+        <f t="shared" si="72"/>
+        <v>Circuit of The Americas</v>
       </c>
       <c r="I104" t="str">
-        <f t="shared" si="77"/>
-        <v>Qatar Grand Prix</v>
+        <f t="shared" si="73"/>
+        <v>Lenovo United States Grand Prix</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C105" t="str">
         <f t="shared" si="1"/>
-        <v>America/Chicago</v>
+        <v>America/Mexico_City</v>
       </c>
       <c r="D105" s="4">
-        <v>45219</v>
-      </c>
-      <c r="E105" s="7">
+        <v>45226</v>
+      </c>
+      <c r="E105" s="5">
         <v>0.52083333333333337</v>
       </c>
       <c r="F105" s="4">
         <f t="shared" si="15"/>
-        <v>45219</v>
+        <v>45226</v>
       </c>
       <c r="G105" s="5">
         <f>E105+(1/24)</f>
         <v>0.5625</v>
       </c>
       <c r="H105" t="str">
-        <f t="shared" si="76"/>
-        <v>Circuit of The Americas</v>
+        <f t="shared" ref="H105:H109" si="78">VLOOKUP(A105,locations,2)</f>
+        <v>Autódromo Hermanos Rodríguez</v>
       </c>
       <c r="I105" t="str">
-        <f t="shared" si="77"/>
-        <v>Lenovo United States Grand Prix</v>
+        <f t="shared" ref="I105:I109" si="79">VLOOKUP(A105,locations,3)</f>
+        <v>Gran Premio de la Ciudad de México</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>11</v>
+        <v>97</v>
       </c>
       <c r="C106" t="str">
         <f t="shared" si="1"/>
-        <v>America/Chicago</v>
+        <v>America/Mexico_City</v>
       </c>
       <c r="D106" s="4">
-        <v>45219</v>
-      </c>
-      <c r="E106" s="7">
+        <v>45226</v>
+      </c>
+      <c r="E106" s="5">
         <v>0.66666666666666663</v>
       </c>
       <c r="F106" s="4">
         <f t="shared" si="15"/>
-        <v>45219</v>
+        <v>45226</v>
       </c>
       <c r="G106" s="5">
         <f t="shared" ref="G106:G108" si="80">E106+(1/24)</f>
         <v>0.70833333333333326</v>
       </c>
       <c r="H106" t="str">
-        <f t="shared" si="76"/>
-        <v>Circuit of The Americas</v>
+        <f t="shared" si="78"/>
+        <v>Autódromo Hermanos Rodríguez</v>
       </c>
       <c r="I106" t="str">
-        <f t="shared" si="77"/>
-        <v>Lenovo United States Grand Prix</v>
+        <f t="shared" si="79"/>
+        <v>Gran Premio de la Ciudad de México</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>141</v>
+        <v>98</v>
       </c>
       <c r="C107" t="str">
         <f t="shared" si="1"/>
-        <v>America/Chicago</v>
+        <v>America/Mexico_City</v>
       </c>
       <c r="D107" s="4">
-        <v>45220</v>
-      </c>
-      <c r="E107" s="7">
+        <v>45227</v>
+      </c>
+      <c r="E107" s="5">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F107" s="4">
+        <f t="shared" si="15"/>
+        <v>45227</v>
+      </c>
+      <c r="G107" s="5">
+        <f t="shared" si="80"/>
         <v>0.52083333333333337</v>
       </c>
-      <c r="F107" s="4">
-        <f t="shared" si="15"/>
-        <v>45220</v>
-      </c>
-      <c r="G107" s="5">
-        <f>E107+(3*(1/96))</f>
-        <v>0.55208333333333337</v>
-      </c>
       <c r="H107" t="str">
-        <f t="shared" si="76"/>
-        <v>Circuit of The Americas</v>
+        <f t="shared" si="78"/>
+        <v>Autódromo Hermanos Rodríguez</v>
       </c>
       <c r="I107" t="str">
-        <f t="shared" si="77"/>
-        <v>Lenovo United States Grand Prix</v>
+        <f t="shared" si="79"/>
+        <v>Gran Premio de la Ciudad de México</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>88</v>
+        <v>11</v>
       </c>
       <c r="C108" t="str">
         <f t="shared" si="1"/>
-        <v>America/Chicago</v>
+        <v>America/Mexico_City</v>
       </c>
       <c r="D108" s="4">
-        <v>45220</v>
+        <v>45227</v>
       </c>
       <c r="E108" s="5">
-        <v>0.70833333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="F108" s="4">
         <f t="shared" si="15"/>
-        <v>45220</v>
+        <v>45227</v>
       </c>
       <c r="G108" s="5">
         <f t="shared" si="80"/>
-        <v>0.75</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="H108" t="str">
-        <f t="shared" si="76"/>
-        <v>Circuit of The Americas</v>
+        <f t="shared" si="78"/>
+        <v>Autódromo Hermanos Rodríguez</v>
       </c>
       <c r="I108" t="str">
-        <f t="shared" si="77"/>
-        <v>Lenovo United States Grand Prix</v>
+        <f t="shared" si="79"/>
+        <v>Gran Premio de la Ciudad de México</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C109" t="str">
         <f t="shared" si="1"/>
-        <v>America/Chicago</v>
+        <v>America/Mexico_City</v>
       </c>
       <c r="D109" s="4">
-        <v>45221</v>
+        <v>45228</v>
       </c>
       <c r="E109" s="5">
         <v>0.58333333333333337</v>
       </c>
       <c r="F109" s="4">
         <f t="shared" si="15"/>
-        <v>45221</v>
+        <v>45228</v>
       </c>
       <c r="G109" s="5">
         <f t="shared" ref="G109" si="81">E109+(2*(1/24))</f>
         <v>0.66666666666666674</v>
       </c>
       <c r="H109" t="str">
-        <f t="shared" si="76"/>
-        <v>Circuit of The Americas</v>
+        <f t="shared" si="78"/>
+        <v>Autódromo Hermanos Rodríguez</v>
       </c>
       <c r="I109" t="str">
-        <f t="shared" si="77"/>
-        <v>Lenovo United States Grand Prix</v>
+        <f t="shared" si="79"/>
+        <v>Gran Premio de la Ciudad de México</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C110" t="str">
         <f t="shared" si="1"/>
-        <v>America/Mexico_City</v>
+        <v>America/Soa_Paulo</v>
       </c>
       <c r="D110" s="4">
-        <v>45226</v>
+        <v>45233</v>
       </c>
       <c r="E110" s="5">
-        <v>0.52083333333333337</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="F110" s="4">
         <f t="shared" si="15"/>
-        <v>45226</v>
+        <v>45233</v>
       </c>
       <c r="G110" s="5">
         <f>E110+(1/24)</f>
-        <v>0.5625</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="H110" t="str">
         <f t="shared" ref="H110:H114" si="82">VLOOKUP(A110,locations,2)</f>
-        <v>Autódromo Hermanos Rodríguez</v>
+        <v>Autódromo José Carlos Pace</v>
       </c>
       <c r="I110" t="str">
         <f t="shared" ref="I110:I114" si="83">VLOOKUP(A110,locations,3)</f>
-        <v>Gran Premio de la Ciudad de México</v>
+        <v>Rolex Grande Prêmio de São Paulo</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>97</v>
+        <v>11</v>
       </c>
       <c r="C111" t="str">
         <f t="shared" si="1"/>
-        <v>America/Mexico_City</v>
+        <v>America/Soa_Paulo</v>
       </c>
       <c r="D111" s="4">
-        <v>45226</v>
+        <v>45233</v>
       </c>
       <c r="E111" s="5">
-        <v>0.66666666666666663</v>
+        <v>0.625</v>
       </c>
       <c r="F111" s="4">
         <f t="shared" si="15"/>
-        <v>45226</v>
+        <v>45233</v>
       </c>
       <c r="G111" s="5">
         <f t="shared" ref="G111:G113" si="84">E111+(1/24)</f>
-        <v>0.70833333333333326</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="H111" t="str">
         <f t="shared" si="82"/>
-        <v>Autódromo Hermanos Rodríguez</v>
+        <v>Autódromo José Carlos Pace</v>
       </c>
       <c r="I111" t="str">
         <f t="shared" si="83"/>
-        <v>Gran Premio de la Ciudad de México</v>
+        <v>Rolex Grande Prêmio de São Paulo</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>98</v>
+        <v>141</v>
       </c>
       <c r="C112" t="str">
         <f t="shared" si="1"/>
-        <v>America/Mexico_City</v>
+        <v>America/Soa_Paulo</v>
       </c>
       <c r="D112" s="4">
-        <v>45227</v>
+        <v>45234</v>
       </c>
       <c r="E112" s="5">
-        <v>0.47916666666666669</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="F112" s="4">
         <f t="shared" si="15"/>
-        <v>45227</v>
+        <v>45234</v>
       </c>
       <c r="G112" s="5">
-        <f t="shared" si="84"/>
-        <v>0.52083333333333337</v>
+        <f>E112+(3*(1/96))</f>
+        <v>0.48958333333333331</v>
       </c>
       <c r="H112" t="str">
         <f t="shared" si="82"/>
-        <v>Autódromo Hermanos Rodríguez</v>
+        <v>Autódromo José Carlos Pace</v>
       </c>
       <c r="I112" t="str">
         <f t="shared" si="83"/>
-        <v>Gran Premio de la Ciudad de México</v>
+        <v>Rolex Grande Prêmio de São Paulo</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="C113" t="str">
-        <f t="shared" si="1"/>
-        <v>America/Mexico_City</v>
+        <f>VLOOKUP(A113,locations,4)</f>
+        <v>America/Soa_Paulo</v>
       </c>
       <c r="D113" s="4">
-        <v>45227</v>
+        <v>45234</v>
       </c>
       <c r="E113" s="5">
-        <v>0.625</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="F113" s="4">
         <f t="shared" si="15"/>
-        <v>45227</v>
+        <v>45234</v>
       </c>
       <c r="G113" s="5">
         <f t="shared" si="84"/>
-        <v>0.66666666666666663</v>
+        <v>0.6875</v>
       </c>
       <c r="H113" t="str">
         <f t="shared" si="82"/>
-        <v>Autódromo Hermanos Rodríguez</v>
+        <v>Autódromo José Carlos Pace</v>
       </c>
       <c r="I113" t="str">
         <f t="shared" si="83"/>
-        <v>Gran Premio de la Ciudad de México</v>
+        <v>Rolex Grande Prêmio de São Paulo</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C114" t="str">
         <f t="shared" si="1"/>
-        <v>America/Mexico_City</v>
+        <v>America/Soa_Paulo</v>
       </c>
       <c r="D114" s="4">
-        <v>45228</v>
+        <v>45235</v>
       </c>
       <c r="E114" s="5">
         <v>0.58333333333333337</v>
       </c>
       <c r="F114" s="4">
         <f t="shared" si="15"/>
-        <v>45228</v>
+        <v>45235</v>
       </c>
       <c r="G114" s="5">
         <f t="shared" ref="G114" si="85">E114+(2*(1/24))</f>
@@ -4711,528 +4709,358 @@
       </c>
       <c r="H114" t="str">
         <f t="shared" si="82"/>
-        <v>Autódromo Hermanos Rodríguez</v>
+        <v>Autódromo José Carlos Pace</v>
       </c>
       <c r="I114" t="str">
         <f t="shared" si="83"/>
-        <v>Gran Premio de la Ciudad de México</v>
+        <v>Rolex Grande Prêmio de São Paulo</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>61</v>
+        <v>111</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C115" t="str">
         <f t="shared" si="1"/>
-        <v>America/Soa_Paulo</v>
+        <v>America/Los_Angeles</v>
       </c>
       <c r="D115" s="4">
-        <v>45233</v>
+        <v>45246</v>
       </c>
       <c r="E115" s="5">
-        <v>0.47916666666666669</v>
+        <v>0.77083333333333337</v>
       </c>
       <c r="F115" s="4">
         <f t="shared" si="15"/>
-        <v>45233</v>
+        <v>45246</v>
       </c>
       <c r="G115" s="5">
         <f>E115+(1/24)</f>
-        <v>0.52083333333333337</v>
+        <v>0.8125</v>
       </c>
       <c r="H115" t="str">
         <f t="shared" ref="H115:H119" si="86">VLOOKUP(A115,locations,2)</f>
-        <v>Autódromo José Carlos Pace</v>
+        <v>Las Vegas</v>
       </c>
       <c r="I115" t="str">
         <f t="shared" ref="I115:I119" si="87">VLOOKUP(A115,locations,3)</f>
-        <v>Rolex Grande Prêmio de São Paulo</v>
+        <v>Heineken Silver Las Vegas Grand Prix</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>61</v>
+        <v>111</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>11</v>
+        <v>97</v>
       </c>
       <c r="C116" t="str">
         <f t="shared" si="1"/>
-        <v>America/Soa_Paulo</v>
+        <v>America/Los_Angeles</v>
       </c>
       <c r="D116" s="4">
-        <v>45233</v>
+        <v>45246</v>
       </c>
       <c r="E116" s="5">
-        <v>0.625</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="F116" s="4">
         <f t="shared" si="15"/>
-        <v>45233</v>
+        <v>45246</v>
       </c>
       <c r="G116" s="5">
         <f t="shared" ref="G116:G118" si="88">E116+(1/24)</f>
-        <v>0.66666666666666663</v>
+        <v>0.95833333333333326</v>
       </c>
       <c r="H116" t="str">
         <f t="shared" si="86"/>
-        <v>Autódromo José Carlos Pace</v>
+        <v>Las Vegas</v>
       </c>
       <c r="I116" t="str">
         <f t="shared" si="87"/>
-        <v>Rolex Grande Prêmio de São Paulo</v>
+        <v>Heineken Silver Las Vegas Grand Prix</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>61</v>
+        <v>111</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>141</v>
+        <v>98</v>
       </c>
       <c r="C117" t="str">
         <f t="shared" si="1"/>
-        <v>America/Soa_Paulo</v>
+        <v>America/Los_Angeles</v>
       </c>
       <c r="D117" s="4">
-        <v>45234</v>
+        <v>45247</v>
       </c>
       <c r="E117" s="5">
-        <v>0.45833333333333331</v>
+        <v>0.77083333333333337</v>
       </c>
       <c r="F117" s="4">
         <f t="shared" si="15"/>
-        <v>45234</v>
+        <v>45247</v>
       </c>
       <c r="G117" s="5">
-        <f>E117+(3*(1/96))</f>
-        <v>0.48958333333333331</v>
+        <f t="shared" si="88"/>
+        <v>0.8125</v>
       </c>
       <c r="H117" t="str">
         <f t="shared" si="86"/>
-        <v>Autódromo José Carlos Pace</v>
+        <v>Las Vegas</v>
       </c>
       <c r="I117" t="str">
         <f t="shared" si="87"/>
-        <v>Rolex Grande Prêmio de São Paulo</v>
+        <v>Heineken Silver Las Vegas Grand Prix</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>61</v>
+        <v>111</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>88</v>
+        <v>11</v>
       </c>
       <c r="C118" t="str">
-        <f>VLOOKUP(A118,locations,4)</f>
-        <v>America/Soa_Paulo</v>
+        <f t="shared" si="1"/>
+        <v>America/Los_Angeles</v>
       </c>
       <c r="D118" s="4">
-        <v>45234</v>
+        <v>45247</v>
       </c>
       <c r="E118" s="5">
-        <v>0.64583333333333337</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="F118" s="4">
         <f t="shared" si="15"/>
-        <v>45234</v>
+        <v>45247</v>
       </c>
       <c r="G118" s="5">
         <f t="shared" si="88"/>
-        <v>0.6875</v>
+        <v>0.95833333333333326</v>
       </c>
       <c r="H118" t="str">
         <f t="shared" si="86"/>
-        <v>Autódromo José Carlos Pace</v>
+        <v>Las Vegas</v>
       </c>
       <c r="I118" t="str">
         <f t="shared" si="87"/>
-        <v>Rolex Grande Prêmio de São Paulo</v>
+        <v>Heineken Silver Las Vegas Grand Prix</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>61</v>
+        <v>111</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C119" t="str">
         <f t="shared" si="1"/>
-        <v>America/Soa_Paulo</v>
+        <v>America/Los_Angeles</v>
       </c>
       <c r="D119" s="4">
-        <v>45235</v>
+        <v>45248</v>
       </c>
       <c r="E119" s="5">
-        <v>0.58333333333333337</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="F119" s="4">
-        <f t="shared" si="15"/>
-        <v>45235</v>
+        <v>45249</v>
       </c>
       <c r="G119" s="5">
         <f t="shared" ref="G119" si="89">E119+(2*(1/24))</f>
-        <v>0.66666666666666674</v>
+        <v>1</v>
       </c>
       <c r="H119" t="str">
         <f t="shared" si="86"/>
-        <v>Autódromo José Carlos Pace</v>
+        <v>Las Vegas</v>
       </c>
       <c r="I119" t="str">
         <f t="shared" si="87"/>
-        <v>Rolex Grande Prêmio de São Paulo</v>
+        <v>Heineken Silver Las Vegas Grand Prix</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C120" t="str">
         <f t="shared" si="1"/>
-        <v>America/Los_Angeles</v>
+        <v>Asia/Qatar</v>
       </c>
       <c r="D120" s="4">
-        <v>45246</v>
+        <v>45254</v>
       </c>
       <c r="E120" s="5">
-        <v>0.77083333333333337</v>
+        <v>0.5625</v>
       </c>
       <c r="F120" s="4">
         <f t="shared" si="15"/>
-        <v>45246</v>
+        <v>45254</v>
       </c>
       <c r="G120" s="5">
         <f>E120+(1/24)</f>
-        <v>0.8125</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="H120" t="str">
-        <f t="shared" ref="H120:H124" si="90">VLOOKUP(A120,locations,2)</f>
-        <v>Las Vegas</v>
+        <f t="shared" ref="H120:H122" si="90">VLOOKUP(A120,locations,2)</f>
+        <v>Yas Marina Circuit</v>
       </c>
       <c r="I120" t="str">
-        <f t="shared" ref="I120:I124" si="91">VLOOKUP(A120,locations,3)</f>
-        <v>Heineken Silver Las Vegas Grand Prix</v>
+        <f t="shared" ref="I120:I122" si="91">VLOOKUP(A120,locations,3)</f>
+        <v>Etihad Airways Abu Dhabi Grand Prix</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>97</v>
       </c>
       <c r="C121" t="str">
         <f t="shared" si="1"/>
-        <v>America/Los_Angeles</v>
+        <v>Asia/Qatar</v>
       </c>
       <c r="D121" s="4">
-        <v>45246</v>
+        <v>45254</v>
       </c>
       <c r="E121" s="5">
-        <v>0.91666666666666663</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="F121" s="4">
         <f t="shared" si="15"/>
-        <v>45246</v>
+        <v>45254</v>
       </c>
       <c r="G121" s="5">
         <f t="shared" ref="G121:G123" si="92">E121+(1/24)</f>
-        <v>0.95833333333333326</v>
+        <v>0.75</v>
       </c>
       <c r="H121" t="str">
         <f t="shared" si="90"/>
-        <v>Las Vegas</v>
+        <v>Yas Marina Circuit</v>
       </c>
       <c r="I121" t="str">
         <f t="shared" si="91"/>
-        <v>Heineken Silver Las Vegas Grand Prix</v>
+        <v>Etihad Airways Abu Dhabi Grand Prix</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>98</v>
       </c>
       <c r="C122" t="str">
         <f t="shared" si="1"/>
-        <v>America/Los_Angeles</v>
+        <v>Asia/Qatar</v>
       </c>
       <c r="D122" s="4">
-        <v>45247</v>
+        <v>45255</v>
       </c>
       <c r="E122" s="5">
-        <v>0.77083333333333337</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="F122" s="4">
         <f t="shared" si="15"/>
-        <v>45247</v>
+        <v>45255</v>
       </c>
       <c r="G122" s="5">
         <f t="shared" si="92"/>
-        <v>0.8125</v>
+        <v>0.64583333333333326</v>
       </c>
       <c r="H122" t="str">
         <f t="shared" si="90"/>
-        <v>Las Vegas</v>
+        <v>Yas Marina Circuit</v>
       </c>
       <c r="I122" t="str">
         <f t="shared" si="91"/>
-        <v>Heineken Silver Las Vegas Grand Prix</v>
+        <v>Etihad Airways Abu Dhabi Grand Prix</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C123" t="str">
         <f t="shared" si="1"/>
-        <v>America/Los_Angeles</v>
+        <v>Asia/Qatar</v>
       </c>
       <c r="D123" s="4">
-        <v>45247</v>
+        <v>45255</v>
       </c>
       <c r="E123" s="5">
-        <v>0.91666666666666663</v>
+        <v>0.75</v>
       </c>
       <c r="F123" s="4">
         <f t="shared" si="15"/>
-        <v>45247</v>
+        <v>45255</v>
       </c>
       <c r="G123" s="5">
         <f t="shared" si="92"/>
-        <v>0.95833333333333326</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="H123" t="str">
-        <f t="shared" si="90"/>
-        <v>Las Vegas</v>
+        <f t="shared" si="16"/>
+        <v>Yas Marina Circuit</v>
       </c>
       <c r="I123" t="str">
-        <f t="shared" si="91"/>
-        <v>Heineken Silver Las Vegas Grand Prix</v>
+        <f t="shared" si="20"/>
+        <v>Etihad Airways Abu Dhabi Grand Prix</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C124" t="str">
         <f t="shared" si="1"/>
-        <v>America/Los_Angeles</v>
+        <v>Asia/Qatar</v>
       </c>
       <c r="D124" s="4">
-        <v>45248</v>
+        <v>45256</v>
       </c>
       <c r="E124" s="5">
-        <v>0.91666666666666663</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="F124" s="4">
-        <v>45249</v>
+        <f t="shared" si="15"/>
+        <v>45256</v>
       </c>
       <c r="G124" s="5">
         <f t="shared" ref="G124" si="93">E124+(2*(1/24))</f>
-        <v>1</v>
+        <v>0.79166666666666674</v>
       </c>
       <c r="H124" t="str">
-        <f t="shared" si="90"/>
-        <v>Las Vegas</v>
+        <f t="shared" ref="H124" si="94">VLOOKUP(A124,locations,2)</f>
+        <v>Yas Marina Circuit</v>
       </c>
       <c r="I124" t="str">
-        <f t="shared" si="91"/>
-        <v>Heineken Silver Las Vegas Grand Prix</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
-        <v>62</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C125" t="str">
-        <f t="shared" si="1"/>
-        <v>Asia/Qatar</v>
-      </c>
-      <c r="D125" s="4">
-        <v>45254</v>
-      </c>
-      <c r="E125" s="5">
-        <v>0.5625</v>
-      </c>
-      <c r="F125" s="4">
-        <f t="shared" si="15"/>
-        <v>45254</v>
-      </c>
-      <c r="G125" s="5">
-        <f>E125+(1/24)</f>
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="H125" t="str">
-        <f t="shared" ref="H125:H127" si="94">VLOOKUP(A125,locations,2)</f>
-        <v>Yas Marina Circuit</v>
-      </c>
-      <c r="I125" t="str">
-        <f t="shared" ref="I125:I127" si="95">VLOOKUP(A125,locations,3)</f>
-        <v>Etihad Airways Abu Dhabi Grand Prix</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
-        <v>62</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C126" t="str">
-        <f t="shared" si="1"/>
-        <v>Asia/Qatar</v>
-      </c>
-      <c r="D126" s="4">
-        <v>45254</v>
-      </c>
-      <c r="E126" s="5">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="F126" s="4">
-        <f t="shared" si="15"/>
-        <v>45254</v>
-      </c>
-      <c r="G126" s="5">
-        <f t="shared" ref="G126:G128" si="96">E126+(1/24)</f>
-        <v>0.75</v>
-      </c>
-      <c r="H126" t="str">
-        <f t="shared" si="94"/>
-        <v>Yas Marina Circuit</v>
-      </c>
-      <c r="I126" t="str">
-        <f t="shared" si="95"/>
-        <v>Etihad Airways Abu Dhabi Grand Prix</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A127" t="s">
-        <v>62</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C127" t="str">
-        <f t="shared" si="1"/>
-        <v>Asia/Qatar</v>
-      </c>
-      <c r="D127" s="4">
-        <v>45255</v>
-      </c>
-      <c r="E127" s="5">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="F127" s="4">
-        <f t="shared" si="15"/>
-        <v>45255</v>
-      </c>
-      <c r="G127" s="5">
-        <f t="shared" si="96"/>
-        <v>0.64583333333333326</v>
-      </c>
-      <c r="H127" t="str">
-        <f t="shared" si="94"/>
-        <v>Yas Marina Circuit</v>
-      </c>
-      <c r="I127" t="str">
-        <f t="shared" si="95"/>
-        <v>Etihad Airways Abu Dhabi Grand Prix</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
-        <v>62</v>
-      </c>
-      <c r="B128" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C128" t="str">
-        <f t="shared" si="1"/>
-        <v>Asia/Qatar</v>
-      </c>
-      <c r="D128" s="4">
-        <v>45255</v>
-      </c>
-      <c r="E128" s="5">
-        <v>0.75</v>
-      </c>
-      <c r="F128" s="4">
-        <f t="shared" si="15"/>
-        <v>45255</v>
-      </c>
-      <c r="G128" s="5">
-        <f t="shared" si="96"/>
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="H128" t="str">
-        <f t="shared" si="16"/>
-        <v>Yas Marina Circuit</v>
-      </c>
-      <c r="I128" t="str">
-        <f t="shared" si="20"/>
-        <v>Etihad Airways Abu Dhabi Grand Prix</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
-        <v>62</v>
-      </c>
-      <c r="B129" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C129" t="str">
-        <f t="shared" si="1"/>
-        <v>Asia/Qatar</v>
-      </c>
-      <c r="D129" s="4">
-        <v>45256</v>
-      </c>
-      <c r="E129" s="5">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="F129" s="4">
-        <f t="shared" si="15"/>
-        <v>45256</v>
-      </c>
-      <c r="G129" s="5">
-        <f t="shared" ref="G129" si="97">E129+(2*(1/24))</f>
-        <v>0.79166666666666674</v>
-      </c>
-      <c r="H129" t="str">
-        <f t="shared" ref="H129" si="98">VLOOKUP(A129,locations,2)</f>
-        <v>Yas Marina Circuit</v>
-      </c>
-      <c r="I129" t="str">
-        <f t="shared" ref="I129" si="99">VLOOKUP(A129,locations,3)</f>
+        <f t="shared" ref="I124" si="95">VLOOKUP(A124,locations,3)</f>
         <v>Etihad Airways Abu Dhabi Grand Prix</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A12:A135" xr:uid="{F03BE25C-DA6F-6246-A9E5-DB905318EDFD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A12:A130" xr:uid="{F03BE25C-DA6F-6246-A9E5-DB905318EDFD}">
       <formula1>countries</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B135" xr:uid="{8F2CDCBC-21D9-4843-9F7D-D70F3A2F785B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B130" xr:uid="{8F2CDCBC-21D9-4843-9F7D-D70F3A2F785B}">
       <formula1>sessions</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update times of Qatar Sprint Shootout and Race
</commit_message>
<xml_diff>
--- a/f1/F1.xlsx
+++ b/f1/F1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin/projects/calendars/f1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7246D45F-FEBD-1A4A-B679-9EC98441A437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2529046-F279-2A48-A3B7-CEEB426465C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3440" yWindow="780" windowWidth="28040" windowHeight="17440" xr2:uid="{65D0735D-D923-6F47-A559-767DB601EBAB}"/>
   </bookViews>
@@ -949,7 +949,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A264AA3C-A8BA-6F48-8FC0-C3E78D3BD742}">
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2657,15 +2659,14 @@
         <v>45206</v>
       </c>
       <c r="E54" s="7">
-        <v>0.5625</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F54" s="4">
         <f t="shared" si="10"/>
         <v>45206</v>
       </c>
       <c r="G54" s="5">
-        <f t="shared" si="61"/>
-        <v>0.60416666666666663</v>
+        <v>0.70138888888888884</v>
       </c>
       <c r="H54" t="str">
         <f t="shared" si="62"/>
@@ -2691,15 +2692,14 @@
         <v>45206</v>
       </c>
       <c r="E55" s="7">
-        <v>0.66666666666666663</v>
+        <v>0.85416666666666663</v>
       </c>
       <c r="F55" s="4">
         <f t="shared" si="10"/>
         <v>45206</v>
       </c>
       <c r="G55" s="5">
-        <f>E55+(3*(1/96))</f>
-        <v>0.69791666666666663</v>
+        <v>0.875</v>
       </c>
       <c r="H55" t="str">
         <f t="shared" si="62"/>

</xml_diff>

<commit_message>
Correct timezone spelling for America/Sao_Paulo
</commit_message>
<xml_diff>
--- a/f1/F1.xlsx
+++ b/f1/F1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin/projects/calendars/f1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2529046-F279-2A48-A3B7-CEEB426465C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF1E8AAA-7ED7-294C-A629-0DF79F0CC57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3440" yWindow="780" windowWidth="28040" windowHeight="17440" xr2:uid="{65D0735D-D923-6F47-A559-767DB601EBAB}"/>
   </bookViews>
@@ -328,9 +328,6 @@
     <t>Ferrari</t>
   </si>
   <si>
-    <t>America/Soa_Paulo</t>
-  </si>
-  <si>
     <t>America/Montreal</t>
   </si>
   <si>
@@ -470,6 +467,9 @@
   </si>
   <si>
     <t>Sprint Shootout</t>
+  </si>
+  <si>
+    <t>America/Sao_Paulo</t>
   </si>
 </sst>
 </file>
@@ -949,9 +949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A264AA3C-A8BA-6F48-8FC0-C3E78D3BD742}">
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -996,7 +994,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>91</v>
@@ -1014,7 +1012,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>91</v>
@@ -1032,7 +1030,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>91</v>
@@ -1050,7 +1048,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>91</v>
@@ -1068,7 +1066,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>91</v>
@@ -1086,7 +1084,7 @@
     </row>
     <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>91</v>
@@ -1155,14 +1153,14 @@
         <v>44971</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F9" s="4">
         <f t="shared" si="0"/>
         <v>44971</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H9"/>
       <c r="I9" t="str">
@@ -1172,7 +1170,7 @@
     </row>
     <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>91</v>
@@ -1201,7 +1199,7 @@
     </row>
     <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>91</v>
@@ -1253,7 +1251,7 @@
         <v>Bahrain International Circuit</v>
       </c>
       <c r="I12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1284,7 +1282,7 @@
         <v>Bahrain International Circuit</v>
       </c>
       <c r="I13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1315,7 +1313,7 @@
         <v>Bahrain International Circuit</v>
       </c>
       <c r="I14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -1561,7 +1559,7 @@
         <v>42</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="1"/>
@@ -1969,7 +1967,7 @@
         <v>18</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C34" t="str">
         <f>VLOOKUP(A34,locations,4)</f>
@@ -2241,7 +2239,7 @@
         <v>57</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="1"/>
@@ -2612,7 +2610,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>11</v>
@@ -2632,7 +2630,7 @@
         <v>45205</v>
       </c>
       <c r="G53" s="5">
-        <f t="shared" ref="G53:G54" si="61">E53+(1/24)</f>
+        <f t="shared" ref="G53" si="61">E53+(1/24)</f>
         <v>0.875</v>
       </c>
       <c r="H53" t="str">
@@ -2646,10 +2644,10 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="1"/>
@@ -2679,7 +2677,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>88</v>
@@ -2712,7 +2710,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>10</v>
@@ -2783,7 +2781,7 @@
         <v>12</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="1"/>
@@ -2957,7 +2955,7 @@
       </c>
       <c r="C63" t="str">
         <f t="shared" si="1"/>
-        <v>America/Soa_Paulo</v>
+        <v>America/Sao_Paulo</v>
       </c>
       <c r="D63" s="4">
         <v>45233</v>
@@ -2987,11 +2985,11 @@
         <v>61</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="1"/>
-        <v>America/Soa_Paulo</v>
+        <v>America/Sao_Paulo</v>
       </c>
       <c r="D64" s="4">
         <v>45234</v>
@@ -3025,7 +3023,7 @@
       </c>
       <c r="C65" t="str">
         <f>VLOOKUP(A65,locations,4)</f>
-        <v>America/Soa_Paulo</v>
+        <v>America/Sao_Paulo</v>
       </c>
       <c r="D65" s="4">
         <v>45234</v>
@@ -3059,7 +3057,7 @@
       </c>
       <c r="C66" t="str">
         <f t="shared" si="1"/>
-        <v>America/Soa_Paulo</v>
+        <v>America/Sao_Paulo</v>
       </c>
       <c r="D66" s="4">
         <v>45235</v>
@@ -3086,7 +3084,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>11</v>
@@ -3120,7 +3118,7 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>10</v>
@@ -3248,9 +3246,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F21C01-9390-E948-88FE-8034CD2A45FB}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3280,10 +3276,10 @@
         <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -3294,7 +3290,7 @@
         <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D2" t="s">
         <v>25</v>
@@ -3303,10 +3299,10 @@
         <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -3317,7 +3313,7 @@
         <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D3" t="s">
         <v>38</v>
@@ -3326,10 +3322,10 @@
         <v>88</v>
       </c>
       <c r="H3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -3346,13 +3342,13 @@
         <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -3375,7 +3371,7 @@
         <v>92</v>
       </c>
       <c r="I5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -3386,19 +3382,19 @@
         <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D6" t="s">
         <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H6" t="s">
         <v>93</v>
       </c>
       <c r="I6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -3415,13 +3411,13 @@
         <v>81</v>
       </c>
       <c r="F7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -3432,19 +3428,19 @@
         <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D8" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="F8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -3458,16 +3454,16 @@
         <v>56</v>
       </c>
       <c r="D9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F9" t="s">
         <v>90</v>
       </c>
       <c r="H9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -3478,7 +3474,7 @@
         <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D10" t="s">
         <v>32</v>
@@ -3487,10 +3483,10 @@
         <v>91</v>
       </c>
       <c r="H10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -3507,10 +3503,10 @@
         <v>31</v>
       </c>
       <c r="H11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -3521,7 +3517,7 @@
         <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D12" t="s">
         <v>35</v>
@@ -3563,7 +3559,7 @@
         <v>76</v>
       </c>
       <c r="C15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D15" t="s">
         <v>37</v>
@@ -3571,16 +3567,16 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" t="s">
         <v>111</v>
       </c>
-      <c r="B16" t="s">
-        <v>111</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>112</v>
-      </c>
-      <c r="D16" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -3605,7 +3601,7 @@
         <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D18" t="s">
         <v>85</v>
@@ -3619,7 +3615,7 @@
         <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D19" t="s">
         <v>31</v>
@@ -3633,7 +3629,7 @@
         <v>70</v>
       </c>
       <c r="C20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D20" t="s">
         <v>89</v>
@@ -3641,13 +3637,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" t="s">
         <v>108</v>
       </c>
-      <c r="B21" t="s">
-        <v>109</v>
-      </c>
       <c r="C21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D21" t="s">
         <v>25</v>
@@ -3675,7 +3671,7 @@
         <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
@@ -3689,7 +3685,7 @@
         <v>75</v>
       </c>
       <c r="C24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D24" t="s">
         <v>87</v>
@@ -3717,7 +3713,7 @@
         <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D26" t="s">
         <v>27</v>

</xml_diff>